<commit_message>
Setting Page + Color
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vocaloid2048\Desktop\File\App\GenshinHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DF82D4-DDB8-4D5E-BA19-AF8924A041F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1397E02B-ED08-41BE-87CE-1139CEE861B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{DB4DA38A-4327-40F6-9D21-54F6AE12F3DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{DB4DA38A-4327-40F6-9D21-54F6AE12F3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Home_List" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2233" uniqueCount="430">
   <si>
     <t>"&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1876,12 +1876,40 @@
     <t xml:space="preserve">String </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>traveler_female</t>
+  </si>
+  <si>
+    <t>traveler_full</t>
+  </si>
+  <si>
+    <t>traveler_anemo</t>
+  </si>
+  <si>
+    <t>traveler_geo</t>
+  </si>
+  <si>
+    <t>traveler_electro</t>
+  </si>
+  <si>
+    <t>Traveler-Anemo</t>
+  </si>
+  <si>
+    <t>Traveler-Geo</t>
+  </si>
+  <si>
+    <t>Traveler-Electro</t>
+  </si>
+  <si>
+    <t>//Add at 210820</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1959,6 +1987,14 @@
       <color rgb="FF3A3A3A"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF9876AA"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2042,7 +2078,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2101,6 +2137,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -7893,10 +7935,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C5A84A-5C7F-451F-A1D8-4D9A74023F1A}">
-  <dimension ref="A1:W87"/>
+  <dimension ref="A1:Y112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -7904,7 +7946,7 @@
     <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>257</v>
       </c>
@@ -7934,45 +7976,52 @@
         <v>aloy_full</v>
       </c>
       <c r="J1" t="s">
+        <v>367</v>
+      </c>
+      <c r="K1" t="str">
+        <f>G1&amp;"_ico"</f>
+        <v>aloy_ico</v>
+      </c>
+      <c r="L1" t="s">
         <v>256</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>368</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>379</v>
       </c>
-      <c r="N1" t="str">
-        <f>L1</f>
+      <c r="P1" t="str">
+        <f>N1</f>
         <v>normal_name</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>401</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>400</v>
       </c>
-      <c r="S1" t="str">
-        <f>Q1</f>
+      <c r="U1" t="str">
+        <f>S1</f>
         <v>sof1_name</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>420</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>401</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>259</v>
       </c>
@@ -8002,45 +8051,52 @@
         <v>kujou_sara_full</v>
       </c>
       <c r="J2" t="s">
+        <v>367</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K45" si="1">G2&amp;"_ico"</f>
+        <v>kujou_sara_ico</v>
+      </c>
+      <c r="L2" t="s">
         <v>256</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>369</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>379</v>
       </c>
-      <c r="N2" t="str">
-        <f t="shared" ref="N2:N11" si="1">L2</f>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P11" si="2">N2</f>
         <v>normal_img</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="Q2" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>402</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>400</v>
       </c>
-      <c r="S2" t="str">
-        <f t="shared" ref="S2:S4" si="2">Q2</f>
+      <c r="U2" t="str">
+        <f t="shared" ref="U2:U4" si="3">S2</f>
         <v>sof1_img</v>
       </c>
-      <c r="T2" s="19" t="s">
+      <c r="V2" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>420</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>402</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>259</v>
       </c>
@@ -8070,45 +8126,52 @@
         <v>sangonomiya_kokomi_full</v>
       </c>
       <c r="J3" t="s">
+        <v>367</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="1"/>
+        <v>sangonomiya_kokomi_ico</v>
+      </c>
+      <c r="L3" t="s">
         <v>256</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>370</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>379</v>
       </c>
-      <c r="N3" t="str">
-        <f t="shared" si="1"/>
+      <c r="P3" t="str">
+        <f t="shared" si="2"/>
         <v>normal_desc1</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="Q3" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>403</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>400</v>
       </c>
-      <c r="S3" t="str">
-        <f t="shared" si="2"/>
+      <c r="U3" t="str">
+        <f t="shared" si="3"/>
         <v>sof1_desc</v>
       </c>
-      <c r="T3" s="19" t="s">
+      <c r="V3" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
         <v>420</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
         <v>403</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>259</v>
       </c>
@@ -8138,45 +8201,52 @@
         <v>raudeb_shougun_full</v>
       </c>
       <c r="J4" t="s">
+        <v>367</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>raudeb_shougun_ico</v>
+      </c>
+      <c r="L4" t="s">
         <v>256</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>371</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>379</v>
       </c>
-      <c r="N4" t="str">
-        <f t="shared" si="1"/>
+      <c r="P4" t="str">
+        <f t="shared" si="2"/>
         <v>normal_desc2</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="Q4" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>404</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>400</v>
       </c>
-      <c r="S4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U4" t="str">
+        <f t="shared" si="3"/>
         <v>sof2_name</v>
       </c>
-      <c r="T4" s="19" t="s">
+      <c r="V4" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U4" t="s">
+      <c r="W4" t="s">
         <v>420</v>
       </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
         <v>404</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Y4" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -8206,45 +8276,52 @@
         <v>sayu_full</v>
       </c>
       <c r="J5" t="s">
+        <v>367</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>sayu_ico</v>
+      </c>
+      <c r="L5" t="s">
         <v>256</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>372</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>379</v>
       </c>
-      <c r="N5" t="str">
-        <f t="shared" si="1"/>
+      <c r="P5" t="str">
+        <f t="shared" si="2"/>
         <v>normal_desc3</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="Q5" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>405</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>400</v>
       </c>
-      <c r="S5" t="str">
-        <f t="shared" ref="S5:S16" si="3">Q5</f>
+      <c r="U5" t="str">
+        <f t="shared" ref="U5:U15" si="4">S5</f>
         <v>sof2_img</v>
       </c>
-      <c r="T5" s="19" t="s">
+      <c r="V5" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U5" t="s">
+      <c r="W5" t="s">
         <v>420</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>405</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Y5" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>259</v>
       </c>
@@ -8274,45 +8351,52 @@
         <v>yoimiya_full</v>
       </c>
       <c r="J6" t="s">
+        <v>367</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>yoimiya_ico</v>
+      </c>
+      <c r="L6" t="s">
         <v>256</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>373</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>379</v>
       </c>
-      <c r="N6" t="str">
-        <f t="shared" si="1"/>
+      <c r="P6" t="str">
+        <f t="shared" si="2"/>
         <v>element_name</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="Q6" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>406</v>
       </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
         <v>400</v>
       </c>
-      <c r="S6" t="str">
-        <f t="shared" si="3"/>
+      <c r="U6" t="str">
+        <f t="shared" si="4"/>
         <v>sof2_desc</v>
       </c>
-      <c r="T6" s="19" t="s">
+      <c r="V6" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>420</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>406</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Y6" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>259</v>
       </c>
@@ -8342,45 +8426,52 @@
         <v>kamisato_ayaka_full</v>
       </c>
       <c r="J7" t="s">
+        <v>367</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>kamisato_ayaka_ico</v>
+      </c>
+      <c r="L7" t="s">
         <v>256</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>374</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>379</v>
       </c>
-      <c r="N7" t="str">
-        <f t="shared" si="1"/>
+      <c r="P7" t="str">
+        <f t="shared" si="2"/>
         <v>element_img</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="Q7" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>407</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>400</v>
       </c>
-      <c r="S7" t="str">
-        <f t="shared" si="3"/>
+      <c r="U7" t="str">
+        <f t="shared" si="4"/>
         <v>sof3_name</v>
       </c>
-      <c r="T7" s="19" t="s">
+      <c r="V7" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U7" t="s">
+      <c r="W7" t="s">
         <v>420</v>
       </c>
-      <c r="V7" t="s">
+      <c r="X7" t="s">
         <v>407</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Y7" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
         <v>259</v>
       </c>
@@ -8410,45 +8501,52 @@
         <v>kaedehara_kazuha_full</v>
       </c>
       <c r="J8" t="s">
+        <v>367</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>kaedehara_kazuha_ico</v>
+      </c>
+      <c r="L8" t="s">
         <v>256</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>375</v>
       </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
         <v>379</v>
       </c>
-      <c r="N8" t="str">
-        <f t="shared" si="1"/>
+      <c r="P8" t="str">
+        <f t="shared" si="2"/>
         <v>element_desc</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="Q8" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
         <v>408</v>
       </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
         <v>400</v>
       </c>
-      <c r="S8" t="str">
-        <f t="shared" si="3"/>
+      <c r="U8" t="str">
+        <f t="shared" si="4"/>
         <v>sof3_img</v>
       </c>
-      <c r="T8" s="19" t="s">
+      <c r="V8" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U8" t="s">
+      <c r="W8" t="s">
         <v>420</v>
       </c>
-      <c r="V8" t="s">
+      <c r="X8" t="s">
         <v>408</v>
       </c>
-      <c r="W8" t="s">
+      <c r="Y8" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
         <v>259</v>
       </c>
@@ -8478,45 +8576,52 @@
         <v>yanfei_full</v>
       </c>
       <c r="J9" t="s">
+        <v>367</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>yanfei_ico</v>
+      </c>
+      <c r="L9" t="s">
         <v>256</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>376</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>379</v>
       </c>
-      <c r="N9" t="str">
-        <f t="shared" si="1"/>
+      <c r="P9" t="str">
+        <f t="shared" si="2"/>
         <v>final_name</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="Q9" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="S9" t="s">
         <v>409</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>400</v>
       </c>
-      <c r="S9" t="str">
-        <f t="shared" si="3"/>
+      <c r="U9" t="str">
+        <f t="shared" si="4"/>
         <v>sof3_desc</v>
       </c>
-      <c r="T9" s="19" t="s">
+      <c r="V9" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U9" t="s">
+      <c r="W9" t="s">
         <v>420</v>
       </c>
-      <c r="V9" t="s">
+      <c r="X9" t="s">
         <v>409</v>
       </c>
-      <c r="W9" t="s">
+      <c r="Y9" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:25">
       <c r="A10" t="s">
         <v>259</v>
       </c>
@@ -8546,45 +8651,52 @@
         <v>eula_full</v>
       </c>
       <c r="J10" t="s">
+        <v>367</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>eula_ico</v>
+      </c>
+      <c r="L10" t="s">
         <v>256</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>377</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>379</v>
       </c>
-      <c r="N10" t="str">
-        <f t="shared" si="1"/>
+      <c r="P10" t="str">
+        <f t="shared" si="2"/>
         <v>final_img</v>
       </c>
-      <c r="O10" s="19" t="s">
+      <c r="Q10" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>410</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>400</v>
       </c>
-      <c r="S10" t="str">
-        <f t="shared" si="3"/>
+      <c r="U10" t="str">
+        <f t="shared" si="4"/>
         <v>sof4_name</v>
       </c>
-      <c r="T10" s="19" t="s">
+      <c r="V10" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U10" t="s">
+      <c r="W10" t="s">
         <v>420</v>
       </c>
-      <c r="V10" t="s">
+      <c r="X10" t="s">
         <v>410</v>
       </c>
-      <c r="W10" t="s">
+      <c r="Y10" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:25">
       <c r="A11" t="s">
         <v>259</v>
       </c>
@@ -8614,45 +8726,52 @@
         <v>rosaria_full</v>
       </c>
       <c r="J11" t="s">
+        <v>367</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>rosaria_ico</v>
+      </c>
+      <c r="L11" t="s">
         <v>256</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>378</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>379</v>
       </c>
-      <c r="N11" t="str">
-        <f t="shared" si="1"/>
+      <c r="P11" t="str">
+        <f t="shared" si="2"/>
         <v>final_desc</v>
       </c>
-      <c r="O11" s="19" t="s">
+      <c r="Q11" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="S11" t="s">
         <v>411</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>400</v>
       </c>
-      <c r="S11" t="str">
-        <f t="shared" si="3"/>
+      <c r="U11" t="str">
+        <f t="shared" si="4"/>
         <v>sof4_img</v>
       </c>
-      <c r="T11" s="19" t="s">
+      <c r="V11" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U11" t="s">
+      <c r="W11" t="s">
         <v>420</v>
       </c>
-      <c r="V11" t="s">
+      <c r="X11" t="s">
         <v>411</v>
       </c>
-      <c r="W11" t="s">
+      <c r="Y11" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:25">
       <c r="A12" t="s">
         <v>259</v>
       </c>
@@ -8682,32 +8801,39 @@
         <v>xiao_full</v>
       </c>
       <c r="J12" t="s">
+        <v>367</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>xiao_ico</v>
+      </c>
+      <c r="L12" t="s">
         <v>256</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
         <v>412</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>400</v>
       </c>
-      <c r="S12" t="str">
-        <f t="shared" si="3"/>
+      <c r="U12" t="str">
+        <f t="shared" si="4"/>
         <v>sof4_desc</v>
       </c>
-      <c r="T12" s="19" t="s">
+      <c r="V12" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U12" t="s">
+      <c r="W12" t="s">
         <v>420</v>
       </c>
-      <c r="V12" t="s">
+      <c r="X12" t="s">
         <v>412</v>
       </c>
-      <c r="W12" t="s">
+      <c r="Y12" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:25">
       <c r="A13" t="s">
         <v>259</v>
       </c>
@@ -8737,45 +8863,52 @@
         <v>hu_tao_full</v>
       </c>
       <c r="J13" t="s">
+        <v>367</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>hu_tao_ico</v>
+      </c>
+      <c r="L13" t="s">
         <v>256</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>384</v>
       </c>
-      <c r="M13" t="s">
+      <c r="O13" t="s">
         <v>381</v>
       </c>
-      <c r="N13" t="str">
-        <f>L13</f>
+      <c r="P13" t="str">
+        <f>N13</f>
         <v>talent1_name</v>
       </c>
-      <c r="O13" s="19" t="s">
+      <c r="Q13" s="19" t="s">
         <v>383</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="S13" t="s">
         <v>413</v>
       </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
         <v>400</v>
       </c>
-      <c r="S13" t="str">
-        <f t="shared" si="3"/>
+      <c r="U13" t="str">
+        <f t="shared" si="4"/>
         <v>sof5_name</v>
       </c>
-      <c r="T13" s="19" t="s">
+      <c r="V13" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U13" t="s">
+      <c r="W13" t="s">
         <v>420</v>
       </c>
-      <c r="V13" t="s">
+      <c r="X13" t="s">
         <v>413</v>
       </c>
-      <c r="W13" t="s">
+      <c r="Y13" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:25">
       <c r="A14" t="s">
         <v>259</v>
       </c>
@@ -8805,45 +8938,52 @@
         <v>ganyu_full</v>
       </c>
       <c r="J14" t="s">
+        <v>367</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>ganyu_ico</v>
+      </c>
+      <c r="L14" t="s">
         <v>256</v>
       </c>
-      <c r="L14" t="s">
+      <c r="N14" t="s">
         <v>385</v>
       </c>
-      <c r="M14" t="s">
+      <c r="O14" t="s">
         <v>382</v>
       </c>
-      <c r="N14" t="str">
-        <f t="shared" ref="N14:N28" si="4">L14</f>
+      <c r="P14" t="str">
+        <f t="shared" ref="P14:P28" si="5">N14</f>
         <v>talent1_unlock</v>
       </c>
-      <c r="O14" s="19" t="s">
+      <c r="Q14" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>414</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
         <v>400</v>
       </c>
-      <c r="S14" t="str">
-        <f t="shared" si="3"/>
+      <c r="U14" t="str">
+        <f t="shared" si="4"/>
         <v>sof5_img</v>
       </c>
-      <c r="T14" s="19" t="s">
+      <c r="V14" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U14" t="s">
+      <c r="W14" t="s">
         <v>420</v>
       </c>
-      <c r="V14" t="s">
+      <c r="X14" t="s">
         <v>414</v>
       </c>
-      <c r="W14" t="s">
+      <c r="Y14" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:25">
       <c r="A15" t="s">
         <v>259</v>
       </c>
@@ -8873,45 +9013,52 @@
         <v>albedo_full</v>
       </c>
       <c r="J15" t="s">
+        <v>367</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>albedo_ico</v>
+      </c>
+      <c r="L15" t="s">
         <v>256</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>386</v>
       </c>
-      <c r="M15" t="s">
+      <c r="O15" t="s">
         <v>381</v>
       </c>
-      <c r="N15" t="str">
+      <c r="P15" t="str">
+        <f t="shared" si="5"/>
+        <v>talent1_img</v>
+      </c>
+      <c r="Q15" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="S15" t="s">
+        <v>415</v>
+      </c>
+      <c r="T15" t="s">
+        <v>400</v>
+      </c>
+      <c r="U15" t="str">
         <f t="shared" si="4"/>
-        <v>talent1_img</v>
-      </c>
-      <c r="O15" s="19" t="s">
+        <v>sof5_desc</v>
+      </c>
+      <c r="V15" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="W15" t="s">
+        <v>420</v>
+      </c>
+      <c r="X15" t="s">
         <v>415</v>
       </c>
-      <c r="R15" t="s">
-        <v>400</v>
-      </c>
-      <c r="S15" t="str">
-        <f t="shared" si="3"/>
-        <v>sof5_desc</v>
-      </c>
-      <c r="T15" s="19" t="s">
-        <v>380</v>
-      </c>
-      <c r="U15" t="s">
-        <v>420</v>
-      </c>
-      <c r="V15" t="s">
-        <v>415</v>
-      </c>
-      <c r="W15" t="s">
+      <c r="Y15" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:25">
       <c r="A16" t="s">
         <v>259</v>
       </c>
@@ -8941,45 +9088,52 @@
         <v>zhongli_full</v>
       </c>
       <c r="J16" t="s">
+        <v>367</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>zhongli_ico</v>
+      </c>
+      <c r="L16" t="s">
         <v>256</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>387</v>
       </c>
-      <c r="M16" t="s">
+      <c r="O16" t="s">
         <v>381</v>
       </c>
-      <c r="N16" t="str">
-        <f t="shared" si="4"/>
+      <c r="P16" t="str">
+        <f t="shared" si="5"/>
         <v>talent1_desc</v>
       </c>
-      <c r="O16" s="19" t="s">
+      <c r="Q16" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
         <v>416</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" t="s">
         <v>400</v>
       </c>
-      <c r="S16" t="str">
-        <f t="shared" ref="S16:S18" si="5">Q16</f>
+      <c r="U16" t="str">
+        <f t="shared" ref="U16:U18" si="6">S16</f>
         <v>sof6_name</v>
       </c>
-      <c r="T16" s="19" t="s">
+      <c r="V16" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U16" t="s">
+      <c r="W16" t="s">
         <v>420</v>
       </c>
-      <c r="V16" t="s">
+      <c r="X16" t="s">
         <v>416</v>
       </c>
-      <c r="W16" t="s">
+      <c r="Y16" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:25">
       <c r="A17" t="s">
         <v>259</v>
       </c>
@@ -9009,45 +9163,52 @@
         <v>xinyan_full</v>
       </c>
       <c r="J17" t="s">
+        <v>367</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>xinyan_ico</v>
+      </c>
+      <c r="L17" t="s">
         <v>256</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>388</v>
       </c>
-      <c r="M17" t="s">
+      <c r="O17" t="s">
         <v>381</v>
       </c>
-      <c r="N17" t="str">
-        <f t="shared" si="4"/>
+      <c r="P17" t="str">
+        <f t="shared" si="5"/>
         <v>talent2_name</v>
       </c>
-      <c r="O17" s="19" t="s">
+      <c r="Q17" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="S17" t="s">
         <v>417</v>
       </c>
-      <c r="R17" t="s">
+      <c r="T17" t="s">
         <v>400</v>
       </c>
-      <c r="S17" t="str">
-        <f t="shared" si="5"/>
+      <c r="U17" t="str">
+        <f t="shared" si="6"/>
         <v>sof6_img</v>
       </c>
-      <c r="T17" s="19" t="s">
+      <c r="V17" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U17" t="s">
+      <c r="W17" t="s">
         <v>420</v>
       </c>
-      <c r="V17" t="s">
+      <c r="X17" t="s">
         <v>417</v>
       </c>
-      <c r="W17" t="s">
+      <c r="Y17" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:25">
       <c r="A18" t="s">
         <v>259</v>
       </c>
@@ -9077,45 +9238,52 @@
         <v>tartaglia_full</v>
       </c>
       <c r="J18" t="s">
+        <v>367</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>tartaglia_ico</v>
+      </c>
+      <c r="L18" t="s">
         <v>256</v>
       </c>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>389</v>
       </c>
-      <c r="M18" t="s">
+      <c r="O18" t="s">
         <v>381</v>
       </c>
-      <c r="N18" t="str">
-        <f t="shared" si="4"/>
+      <c r="P18" t="str">
+        <f t="shared" si="5"/>
         <v>talent2_unlock</v>
       </c>
-      <c r="O18" s="19" t="s">
+      <c r="Q18" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="S18" t="s">
         <v>418</v>
       </c>
-      <c r="R18" t="s">
+      <c r="T18" t="s">
         <v>400</v>
       </c>
-      <c r="S18" t="str">
-        <f t="shared" si="5"/>
+      <c r="U18" t="str">
+        <f t="shared" si="6"/>
         <v>sof6_desc</v>
       </c>
-      <c r="T18" s="19" t="s">
+      <c r="V18" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="U18" t="s">
+      <c r="W18" t="s">
         <v>420</v>
       </c>
-      <c r="V18" t="s">
+      <c r="X18" t="s">
         <v>418</v>
       </c>
-      <c r="W18" t="s">
+      <c r="Y18" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:25">
       <c r="A19" t="s">
         <v>259</v>
       </c>
@@ -9145,23 +9313,30 @@
         <v>diona_full</v>
       </c>
       <c r="J19" t="s">
+        <v>367</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>diona_ico</v>
+      </c>
+      <c r="L19" t="s">
         <v>256</v>
       </c>
-      <c r="L19" t="s">
+      <c r="N19" t="s">
         <v>390</v>
       </c>
-      <c r="M19" t="s">
+      <c r="O19" t="s">
         <v>381</v>
       </c>
-      <c r="N19" t="str">
-        <f t="shared" si="4"/>
+      <c r="P19" t="str">
+        <f t="shared" si="5"/>
         <v>talent2_img</v>
       </c>
-      <c r="O19" s="19" t="s">
+      <c r="Q19" s="19" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:25">
       <c r="A20" t="s">
         <v>259</v>
       </c>
@@ -9191,23 +9366,30 @@
         <v>xingqiu_full</v>
       </c>
       <c r="J20" t="s">
+        <v>367</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>xingqiu_ico</v>
+      </c>
+      <c r="L20" t="s">
         <v>256</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>391</v>
       </c>
-      <c r="M20" t="s">
+      <c r="O20" t="s">
         <v>381</v>
       </c>
-      <c r="N20" t="str">
-        <f t="shared" si="4"/>
+      <c r="P20" t="str">
+        <f t="shared" si="5"/>
         <v>talent2_desc</v>
       </c>
-      <c r="O20" s="19" t="s">
+      <c r="Q20" s="19" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:25">
       <c r="A21" t="s">
         <v>259</v>
       </c>
@@ -9237,23 +9419,30 @@
         <v>xiangling_full</v>
       </c>
       <c r="J21" t="s">
+        <v>367</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>xiangling_ico</v>
+      </c>
+      <c r="L21" t="s">
         <v>256</v>
       </c>
-      <c r="L21" t="s">
+      <c r="N21" t="s">
         <v>392</v>
       </c>
-      <c r="M21" t="s">
+      <c r="O21" t="s">
         <v>381</v>
       </c>
-      <c r="N21" t="str">
-        <f t="shared" si="4"/>
+      <c r="P21" t="str">
+        <f t="shared" si="5"/>
         <v>talent3_name</v>
       </c>
-      <c r="O21" s="19" t="s">
+      <c r="Q21" s="19" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:25">
       <c r="A22" t="s">
         <v>259</v>
       </c>
@@ -9283,23 +9472,30 @@
         <v>venti_full</v>
       </c>
       <c r="J22" t="s">
+        <v>367</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>venti_ico</v>
+      </c>
+      <c r="L22" t="s">
         <v>256</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>393</v>
       </c>
-      <c r="M22" t="s">
+      <c r="O22" t="s">
         <v>381</v>
       </c>
-      <c r="N22" t="str">
-        <f t="shared" si="4"/>
+      <c r="P22" t="str">
+        <f t="shared" si="5"/>
         <v>talent3_unlock</v>
       </c>
-      <c r="O22" s="19" t="s">
+      <c r="Q22" s="19" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:25">
       <c r="A23" t="s">
         <v>259</v>
       </c>
@@ -9329,23 +9525,30 @@
         <v>traveler_full</v>
       </c>
       <c r="J23" t="s">
+        <v>367</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>traveler_ico</v>
+      </c>
+      <c r="L23" t="s">
         <v>256</v>
       </c>
-      <c r="L23" t="s">
+      <c r="N23" t="s">
         <v>394</v>
       </c>
-      <c r="M23" t="s">
+      <c r="O23" t="s">
         <v>381</v>
       </c>
-      <c r="N23" t="str">
-        <f t="shared" si="4"/>
+      <c r="P23" t="str">
+        <f t="shared" si="5"/>
         <v>talent3_img</v>
       </c>
-      <c r="O23" s="19" t="s">
+      <c r="Q23" s="19" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:25">
       <c r="A24" t="s">
         <v>259</v>
       </c>
@@ -9375,23 +9578,30 @@
         <v>sucrose_full</v>
       </c>
       <c r="J24" t="s">
+        <v>367</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>sucrose_ico</v>
+      </c>
+      <c r="L24" t="s">
         <v>256</v>
       </c>
-      <c r="L24" t="s">
+      <c r="N24" t="s">
         <v>395</v>
       </c>
-      <c r="M24" t="s">
+      <c r="O24" t="s">
         <v>381</v>
       </c>
-      <c r="N24" t="str">
-        <f t="shared" si="4"/>
+      <c r="P24" t="str">
+        <f t="shared" si="5"/>
         <v>talent3_desc</v>
       </c>
-      <c r="O24" s="19" t="s">
+      <c r="Q24" s="19" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:25">
       <c r="A25" t="s">
         <v>259</v>
       </c>
@@ -9421,23 +9631,30 @@
         <v>razor_full</v>
       </c>
       <c r="J25" t="s">
+        <v>367</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>razor_ico</v>
+      </c>
+      <c r="L25" t="s">
         <v>256</v>
       </c>
-      <c r="L25" t="s">
+      <c r="N25" t="s">
         <v>396</v>
       </c>
-      <c r="M25" t="s">
+      <c r="O25" t="s">
         <v>381</v>
       </c>
-      <c r="N25" t="str">
-        <f t="shared" si="4"/>
+      <c r="P25" t="str">
+        <f t="shared" si="5"/>
         <v>talent4_name</v>
       </c>
-      <c r="O25" s="19" t="s">
+      <c r="Q25" s="19" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:25">
       <c r="A26" t="s">
         <v>259</v>
       </c>
@@ -9467,23 +9684,30 @@
         <v>qiqi_full</v>
       </c>
       <c r="J26" t="s">
+        <v>367</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>qiqi_ico</v>
+      </c>
+      <c r="L26" t="s">
         <v>256</v>
       </c>
-      <c r="L26" t="s">
+      <c r="N26" t="s">
         <v>397</v>
       </c>
-      <c r="M26" t="s">
+      <c r="O26" t="s">
         <v>381</v>
       </c>
-      <c r="N26" t="str">
-        <f t="shared" si="4"/>
+      <c r="P26" t="str">
+        <f t="shared" si="5"/>
         <v>talent4_unlock</v>
       </c>
-      <c r="O26" s="19" t="s">
+      <c r="Q26" s="19" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:25">
       <c r="A27" t="s">
         <v>259</v>
       </c>
@@ -9513,23 +9737,30 @@
         <v>noelle_full</v>
       </c>
       <c r="J27" t="s">
+        <v>367</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>noelle_ico</v>
+      </c>
+      <c r="L27" t="s">
         <v>256</v>
       </c>
-      <c r="L27" t="s">
+      <c r="N27" t="s">
         <v>398</v>
       </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
         <v>381</v>
       </c>
-      <c r="N27" t="str">
-        <f t="shared" si="4"/>
+      <c r="P27" t="str">
+        <f t="shared" si="5"/>
         <v>talent4_img</v>
       </c>
-      <c r="O27" s="19" t="s">
+      <c r="Q27" s="19" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:25">
       <c r="A28" t="s">
         <v>259</v>
       </c>
@@ -9559,23 +9790,30 @@
         <v>ningguang_full</v>
       </c>
       <c r="J28" t="s">
+        <v>367</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>ningguang_ico</v>
+      </c>
+      <c r="L28" t="s">
         <v>256</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>399</v>
       </c>
-      <c r="M28" t="s">
+      <c r="O28" t="s">
         <v>381</v>
       </c>
-      <c r="N28" t="str">
-        <f t="shared" si="4"/>
+      <c r="P28" t="str">
+        <f t="shared" si="5"/>
         <v>talent4_desc</v>
       </c>
-      <c r="O28" s="19" t="s">
+      <c r="Q28" s="19" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:25">
       <c r="A29" t="s">
         <v>259</v>
       </c>
@@ -9605,10 +9843,17 @@
         <v>mona_full</v>
       </c>
       <c r="J29" t="s">
+        <v>367</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>mona_ico</v>
+      </c>
+      <c r="L29" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:25">
       <c r="A30" t="s">
         <v>259</v>
       </c>
@@ -9638,10 +9883,17 @@
         <v>lisa_full</v>
       </c>
       <c r="J30" t="s">
+        <v>367</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>lisa_ico</v>
+      </c>
+      <c r="L30" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:25">
       <c r="A31" t="s">
         <v>259</v>
       </c>
@@ -9671,10 +9923,17 @@
         <v>klee_full</v>
       </c>
       <c r="J31" t="s">
+        <v>367</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>klee_ico</v>
+      </c>
+      <c r="L31" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:25">
       <c r="A32" t="s">
         <v>259</v>
       </c>
@@ -9704,10 +9963,17 @@
         <v>keqing_full</v>
       </c>
       <c r="J32" t="s">
+        <v>367</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>keqing_ico</v>
+      </c>
+      <c r="L32" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>259</v>
       </c>
@@ -9737,10 +10003,17 @@
         <v>kaeya_full</v>
       </c>
       <c r="J33" t="s">
+        <v>367</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>kaeya_ico</v>
+      </c>
+      <c r="L33" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>259</v>
       </c>
@@ -9770,10 +10043,17 @@
         <v>jean_full</v>
       </c>
       <c r="J34" t="s">
+        <v>367</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>jean_ico</v>
+      </c>
+      <c r="L34" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>259</v>
       </c>
@@ -9803,10 +10083,17 @@
         <v>fischl_full</v>
       </c>
       <c r="J35" t="s">
+        <v>367</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>fischl_ico</v>
+      </c>
+      <c r="L35" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>259</v>
       </c>
@@ -9836,10 +10123,17 @@
         <v>diluc_full</v>
       </c>
       <c r="J36" t="s">
+        <v>367</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v>diluc_ico</v>
+      </c>
+      <c r="L36" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>259</v>
       </c>
@@ -9869,10 +10163,17 @@
         <v>chongyun_full</v>
       </c>
       <c r="J37" t="s">
+        <v>367</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v>chongyun_ico</v>
+      </c>
+      <c r="L37" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>259</v>
       </c>
@@ -9902,10 +10203,17 @@
         <v>bennett_full</v>
       </c>
       <c r="J38" t="s">
+        <v>367</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="1"/>
+        <v>bennett_ico</v>
+      </c>
+      <c r="L38" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>259</v>
       </c>
@@ -9935,10 +10243,17 @@
         <v>beidou_full</v>
       </c>
       <c r="J39" t="s">
+        <v>367</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="1"/>
+        <v>beidou_ico</v>
+      </c>
+      <c r="L39" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>259</v>
       </c>
@@ -9968,10 +10283,17 @@
         <v>barbara_full</v>
       </c>
       <c r="J40" t="s">
+        <v>367</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="1"/>
+        <v>barbara_ico</v>
+      </c>
+      <c r="L40" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>259</v>
       </c>
@@ -10001,1088 +10323,1344 @@
         <v>amber_full</v>
       </c>
       <c r="J41" t="s">
+        <v>367</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="1"/>
+        <v>amber_ico</v>
+      </c>
+      <c r="L41" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
-      <c r="B44" t="s">
+    <row r="42" spans="1:12">
+      <c r="A42" t="s">
+        <v>429</v>
+      </c>
+      <c r="B42" s="20"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" t="s">
+        <v>259</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>426</v>
+      </c>
+      <c r="C43" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" t="s">
+        <v>171</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="F43" t="s">
+        <v>172</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>423</v>
+      </c>
+      <c r="H43" t="s">
+        <v>367</v>
+      </c>
+      <c r="I43" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="J43" t="s">
+        <v>367</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="1"/>
+        <v>traveler_anemo_ico</v>
+      </c>
+      <c r="L43" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" t="s">
+        <v>259</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>427</v>
+      </c>
+      <c r="C44" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" t="s">
+        <v>171</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="F44" t="s">
+        <v>172</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="H44" t="s">
+        <v>367</v>
+      </c>
+      <c r="I44" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="J44" t="s">
+        <v>367</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="1"/>
+        <v>traveler_geo_ico</v>
+      </c>
+      <c r="L44" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" t="s">
+        <v>259</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="C45" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" t="s">
+        <v>171</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="F45" t="s">
+        <v>172</v>
+      </c>
+      <c r="G45" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="H45" t="s">
+        <v>367</v>
+      </c>
+      <c r="I45" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="J45" t="s">
+        <v>367</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="1"/>
+        <v>traveler_electro_ico</v>
+      </c>
+      <c r="L45" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="B46" s="19"/>
+      <c r="E46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="I46" s="21"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="B47" s="19"/>
+      <c r="E47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="I47" s="21"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="B48" s="19"/>
+      <c r="E48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="I48" s="21"/>
+    </row>
+    <row r="49" spans="2:9">
+      <c r="B49" s="19"/>
+      <c r="E49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="I49" s="21"/>
+    </row>
+    <row r="50" spans="2:9">
+      <c r="B50" s="19"/>
+      <c r="E50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="I50" s="21"/>
+    </row>
+    <row r="51" spans="2:9">
+      <c r="B51" s="19"/>
+      <c r="E51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="I51" s="21"/>
+    </row>
+    <row r="52" spans="2:9">
+      <c r="B52" s="19"/>
+      <c r="E52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="I52" s="21"/>
+    </row>
+    <row r="53" spans="2:9">
+      <c r="B53" s="19"/>
+      <c r="E53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="I53" s="21"/>
+    </row>
+    <row r="54" spans="2:9">
+      <c r="B54" s="19"/>
+      <c r="E54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="I54" s="21"/>
+    </row>
+    <row r="55" spans="2:9">
+      <c r="B55" s="19"/>
+      <c r="E55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="I55" s="21"/>
+    </row>
+    <row r="56" spans="2:9">
+      <c r="B56" s="19"/>
+      <c r="E56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="I56" s="21"/>
+    </row>
+    <row r="57" spans="2:9">
+      <c r="B57" s="19"/>
+      <c r="E57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="I57" s="21"/>
+    </row>
+    <row r="58" spans="2:9">
+      <c r="B58" s="19"/>
+      <c r="E58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="I58" s="21"/>
+    </row>
+    <row r="59" spans="2:9">
+      <c r="B59" s="19"/>
+      <c r="E59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="I59" s="21"/>
+    </row>
+    <row r="60" spans="2:9">
+      <c r="B60" s="19"/>
+      <c r="E60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="I60" s="21"/>
+    </row>
+    <row r="61" spans="2:9">
+      <c r="B61" s="19"/>
+      <c r="E61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="I61" s="21"/>
+    </row>
+    <row r="62" spans="2:9">
+      <c r="B62" s="19"/>
+      <c r="E62" s="21"/>
+      <c r="G62" s="21"/>
+      <c r="I62" s="21"/>
+    </row>
+    <row r="63" spans="2:9">
+      <c r="B63" s="19"/>
+      <c r="E63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="I63" s="21"/>
+    </row>
+    <row r="64" spans="2:9">
+      <c r="B64" s="19"/>
+      <c r="E64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="I64" s="21"/>
+    </row>
+    <row r="65" spans="1:15">
+      <c r="B65" s="19"/>
+      <c r="E65" s="21"/>
+      <c r="G65" s="21"/>
+      <c r="I65" s="21"/>
+    </row>
+    <row r="66" spans="1:15">
+      <c r="B66" s="19"/>
+      <c r="E66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="I66" s="21"/>
+    </row>
+    <row r="69" spans="1:15">
+      <c r="B69" t="s">
         <v>260</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C69" t="s">
         <v>261</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D69" t="s">
         <v>260</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E69" t="s">
         <v>262</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F69" t="s">
         <v>260</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G69" t="s">
         <v>263</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H69" t="s">
         <v>260</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I69" t="s">
         <v>264</v>
       </c>
-      <c r="J44" t="s">
+      <c r="L69" t="s">
         <v>260</v>
       </c>
-      <c r="K44" t="s">
+      <c r="M69" t="s">
         <v>265</v>
       </c>
-      <c r="L44" t="s">
+      <c r="N69" t="s">
         <v>260</v>
       </c>
-      <c r="M44" t="s">
+      <c r="O69" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
-      <c r="B45" t="s">
+    <row r="70" spans="1:15">
+      <c r="B70" t="s">
         <v>267</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C70" t="s">
         <v>261</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D70" t="s">
         <v>260</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E70" t="s">
         <v>262</v>
       </c>
-      <c r="F45" t="str">
-        <f>$B45</f>
+      <c r="F70" t="str">
+        <f>$B70</f>
         <v>hydro</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G70" t="s">
         <v>263</v>
       </c>
-      <c r="H45" t="str">
-        <f>$B45</f>
+      <c r="H70" t="str">
+        <f>$B70</f>
         <v>hydro</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I70" t="s">
         <v>264</v>
       </c>
-      <c r="J45" t="str">
-        <f>$B45</f>
+      <c r="L70" t="str">
+        <f>$B70</f>
         <v>hydro</v>
       </c>
-      <c r="K45" t="s">
+      <c r="M70" t="s">
         <v>265</v>
       </c>
-      <c r="L45" t="str">
-        <f>$B45</f>
+      <c r="N70" t="str">
+        <f>$B70</f>
         <v>hydro</v>
       </c>
-      <c r="M45" t="s">
+      <c r="O70" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
-      <c r="B46" t="s">
+    <row r="71" spans="1:15">
+      <c r="B71" t="s">
         <v>268</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C71" t="s">
         <v>261</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D71" t="s">
         <v>260</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E71" t="s">
         <v>262</v>
       </c>
-      <c r="F46" t="str">
-        <f t="shared" ref="F46:L55" si="6">$B46</f>
+      <c r="F71" t="str">
+        <f t="shared" ref="F71:N80" si="7">$B71</f>
         <v>anemo</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G71" t="s">
         <v>263</v>
       </c>
-      <c r="H46" t="str">
-        <f t="shared" si="6"/>
+      <c r="H71" t="str">
+        <f t="shared" si="7"/>
         <v>anemo</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I71" t="s">
         <v>264</v>
       </c>
-      <c r="J46" t="str">
-        <f t="shared" si="6"/>
+      <c r="L71" t="str">
+        <f t="shared" si="7"/>
         <v>anemo</v>
       </c>
-      <c r="K46" t="s">
+      <c r="M71" t="s">
         <v>265</v>
       </c>
-      <c r="L46" t="str">
-        <f t="shared" si="6"/>
+      <c r="N71" t="str">
+        <f t="shared" si="7"/>
         <v>anemo</v>
       </c>
-      <c r="M46" t="s">
+      <c r="O71" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
-      <c r="B47" t="s">
+    <row r="72" spans="1:15">
+      <c r="B72" t="s">
         <v>269</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C72" t="s">
         <v>261</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D72" t="s">
         <v>260</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E72" t="s">
         <v>262</v>
       </c>
-      <c r="F47" t="str">
-        <f t="shared" si="6"/>
+      <c r="F72" t="str">
+        <f t="shared" si="7"/>
         <v>electro</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G72" t="s">
         <v>263</v>
       </c>
-      <c r="H47" t="str">
-        <f t="shared" si="6"/>
+      <c r="H72" t="str">
+        <f t="shared" si="7"/>
         <v>electro</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I72" t="s">
         <v>264</v>
       </c>
-      <c r="J47" t="str">
-        <f t="shared" si="6"/>
+      <c r="L72" t="str">
+        <f t="shared" si="7"/>
         <v>electro</v>
       </c>
-      <c r="K47" t="s">
+      <c r="M72" t="s">
         <v>265</v>
       </c>
-      <c r="L47" t="str">
-        <f t="shared" si="6"/>
+      <c r="N72" t="str">
+        <f t="shared" si="7"/>
         <v>electro</v>
       </c>
-      <c r="M47" t="s">
+      <c r="O72" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
-      <c r="B48" t="s">
+    <row r="73" spans="1:15">
+      <c r="B73" t="s">
         <v>270</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C73" t="s">
         <v>261</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D73" t="s">
         <v>260</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E73" t="s">
         <v>262</v>
       </c>
-      <c r="F48" t="str">
-        <f t="shared" si="6"/>
+      <c r="F73" t="str">
+        <f t="shared" si="7"/>
         <v>dendor</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G73" t="s">
         <v>263</v>
       </c>
-      <c r="H48" t="str">
-        <f t="shared" si="6"/>
+      <c r="H73" t="str">
+        <f t="shared" si="7"/>
         <v>dendor</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I73" t="s">
         <v>264</v>
       </c>
-      <c r="J48" t="str">
-        <f t="shared" si="6"/>
+      <c r="L73" t="str">
+        <f t="shared" si="7"/>
         <v>dendor</v>
       </c>
-      <c r="K48" t="s">
+      <c r="M73" t="s">
         <v>265</v>
       </c>
-      <c r="L48" t="str">
-        <f t="shared" si="6"/>
+      <c r="N73" t="str">
+        <f t="shared" si="7"/>
         <v>dendor</v>
       </c>
-      <c r="M48" t="s">
+      <c r="O73" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
-      <c r="B49" t="s">
+    <row r="74" spans="1:15">
+      <c r="B74" t="s">
         <v>271</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C74" t="s">
         <v>261</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D74" t="s">
         <v>260</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E74" t="s">
         <v>262</v>
       </c>
-      <c r="F49" t="str">
-        <f t="shared" si="6"/>
+      <c r="F74" t="str">
+        <f t="shared" si="7"/>
         <v>cryo</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G74" t="s">
         <v>263</v>
       </c>
-      <c r="H49" t="str">
-        <f t="shared" si="6"/>
+      <c r="H74" t="str">
+        <f t="shared" si="7"/>
         <v>cryo</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I74" t="s">
         <v>264</v>
       </c>
-      <c r="J49" t="str">
-        <f t="shared" si="6"/>
+      <c r="L74" t="str">
+        <f t="shared" si="7"/>
         <v>cryo</v>
       </c>
-      <c r="K49" t="s">
+      <c r="M74" t="s">
         <v>265</v>
       </c>
-      <c r="L49" t="str">
-        <f t="shared" si="6"/>
+      <c r="N74" t="str">
+        <f t="shared" si="7"/>
         <v>cryo</v>
       </c>
-      <c r="M49" t="s">
+      <c r="O74" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
-      <c r="B50" t="s">
+    <row r="75" spans="1:15">
+      <c r="B75" t="s">
         <v>272</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C75" t="s">
         <v>261</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D75" t="s">
         <v>260</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E75" t="s">
         <v>262</v>
       </c>
-      <c r="F50" t="str">
-        <f t="shared" si="6"/>
+      <c r="F75" t="str">
+        <f t="shared" si="7"/>
         <v>geo</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G75" t="s">
         <v>263</v>
       </c>
-      <c r="H50" t="str">
-        <f t="shared" si="6"/>
+      <c r="H75" t="str">
+        <f t="shared" si="7"/>
         <v>geo</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I75" t="s">
         <v>264</v>
       </c>
-      <c r="J50" t="str">
-        <f t="shared" si="6"/>
+      <c r="L75" t="str">
+        <f t="shared" si="7"/>
         <v>geo</v>
       </c>
-      <c r="K50" t="s">
+      <c r="M75" t="s">
         <v>265</v>
       </c>
-      <c r="L50" t="str">
-        <f t="shared" si="6"/>
+      <c r="N75" t="str">
+        <f t="shared" si="7"/>
         <v>geo</v>
       </c>
-      <c r="M50" t="s">
+      <c r="O75" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
-      <c r="A51" t="s">
+    <row r="76" spans="1:15">
+      <c r="A76" t="s">
         <v>273</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B76" t="s">
         <v>274</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C76" t="s">
         <v>261</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D76" t="s">
         <v>260</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E76" t="s">
         <v>262</v>
       </c>
-      <c r="F51" t="str">
-        <f t="shared" si="6"/>
+      <c r="F76" t="str">
+        <f t="shared" si="7"/>
         <v>sword</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G76" t="s">
         <v>263</v>
       </c>
-      <c r="H51" t="str">
-        <f>$A51&amp;$B51</f>
+      <c r="H76" t="str">
+        <f>$A76&amp;$B76</f>
         <v>ico_sword</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I76" t="s">
         <v>264</v>
       </c>
-      <c r="J51" t="str">
-        <f t="shared" si="6"/>
+      <c r="L76" t="str">
+        <f t="shared" si="7"/>
         <v>sword</v>
       </c>
-      <c r="K51" t="s">
+      <c r="M76" t="s">
         <v>265</v>
       </c>
-      <c r="L51" t="str">
-        <f>$A51&amp;$B51</f>
+      <c r="N76" t="str">
+        <f>$A76&amp;$B76</f>
         <v>ico_sword</v>
       </c>
-      <c r="M51" t="s">
+      <c r="O76" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
-      <c r="A52" t="s">
+    <row r="77" spans="1:15">
+      <c r="A77" t="s">
         <v>273</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B77" t="s">
         <v>275</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C77" t="s">
         <v>261</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D77" t="s">
         <v>260</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E77" t="s">
         <v>262</v>
       </c>
-      <c r="F52" t="str">
-        <f t="shared" si="6"/>
+      <c r="F77" t="str">
+        <f t="shared" si="7"/>
         <v>claymore</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G77" t="s">
         <v>263</v>
       </c>
-      <c r="H52" t="str">
-        <f t="shared" ref="H52:H55" si="7">$A52&amp;$B52</f>
+      <c r="H77" t="str">
+        <f t="shared" ref="H77:H80" si="8">$A77&amp;$B77</f>
         <v>ico_claymore</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I77" t="s">
         <v>264</v>
       </c>
-      <c r="J52" t="str">
-        <f t="shared" si="6"/>
+      <c r="L77" t="str">
+        <f t="shared" si="7"/>
         <v>claymore</v>
       </c>
-      <c r="K52" t="s">
+      <c r="M77" t="s">
         <v>265</v>
       </c>
-      <c r="L52" t="str">
-        <f t="shared" ref="L52:L55" si="8">$A52&amp;$B52</f>
+      <c r="N77" t="str">
+        <f t="shared" ref="N77:N80" si="9">$A77&amp;$B77</f>
         <v>ico_claymore</v>
       </c>
-      <c r="M52" t="s">
+      <c r="O77" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
-      <c r="A53" t="s">
+    <row r="78" spans="1:15">
+      <c r="A78" t="s">
         <v>273</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B78" t="s">
         <v>276</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C78" t="s">
         <v>261</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D78" t="s">
         <v>260</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E78" t="s">
         <v>262</v>
       </c>
-      <c r="F53" t="str">
-        <f t="shared" si="6"/>
+      <c r="F78" t="str">
+        <f t="shared" si="7"/>
         <v>polearm</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G78" t="s">
         <v>263</v>
       </c>
-      <c r="H53" t="str">
-        <f t="shared" si="7"/>
-        <v>ico_polearm</v>
-      </c>
-      <c r="I53" t="s">
-        <v>264</v>
-      </c>
-      <c r="J53" t="str">
-        <f t="shared" si="6"/>
-        <v>polearm</v>
-      </c>
-      <c r="K53" t="s">
-        <v>265</v>
-      </c>
-      <c r="L53" t="str">
+      <c r="H78" t="str">
         <f t="shared" si="8"/>
         <v>ico_polearm</v>
       </c>
-      <c r="M53" t="s">
+      <c r="I78" t="s">
+        <v>264</v>
+      </c>
+      <c r="L78" t="str">
+        <f t="shared" si="7"/>
+        <v>polearm</v>
+      </c>
+      <c r="M78" t="s">
+        <v>265</v>
+      </c>
+      <c r="N78" t="str">
+        <f t="shared" si="9"/>
+        <v>ico_polearm</v>
+      </c>
+      <c r="O78" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
-      <c r="A54" t="s">
+    <row r="79" spans="1:15">
+      <c r="A79" t="s">
         <v>273</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B79" t="s">
         <v>277</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C79" t="s">
         <v>261</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D79" t="s">
         <v>260</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E79" t="s">
         <v>262</v>
       </c>
-      <c r="F54" t="str">
-        <f t="shared" si="6"/>
+      <c r="F79" t="str">
+        <f t="shared" si="7"/>
         <v>bow</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G79" t="s">
         <v>263</v>
       </c>
-      <c r="H54" t="str">
-        <f t="shared" si="7"/>
-        <v>ico_bow</v>
-      </c>
-      <c r="I54" t="s">
-        <v>264</v>
-      </c>
-      <c r="J54" t="str">
-        <f t="shared" si="6"/>
-        <v>bow</v>
-      </c>
-      <c r="K54" t="s">
-        <v>265</v>
-      </c>
-      <c r="L54" t="str">
+      <c r="H79" t="str">
         <f t="shared" si="8"/>
         <v>ico_bow</v>
       </c>
-      <c r="M54" t="s">
+      <c r="I79" t="s">
+        <v>264</v>
+      </c>
+      <c r="L79" t="str">
+        <f t="shared" si="7"/>
+        <v>bow</v>
+      </c>
+      <c r="M79" t="s">
+        <v>265</v>
+      </c>
+      <c r="N79" t="str">
+        <f t="shared" si="9"/>
+        <v>ico_bow</v>
+      </c>
+      <c r="O79" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
-      <c r="A55" t="s">
+    <row r="80" spans="1:15">
+      <c r="A80" t="s">
         <v>273</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B80" t="s">
         <v>278</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C80" t="s">
         <v>261</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D80" t="s">
         <v>260</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E80" t="s">
         <v>262</v>
       </c>
-      <c r="F55" t="str">
-        <f t="shared" si="6"/>
+      <c r="F80" t="str">
+        <f t="shared" si="7"/>
         <v>catalyst</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G80" t="s">
         <v>263</v>
       </c>
-      <c r="H55" t="str">
-        <f t="shared" si="7"/>
-        <v>ico_catalyst</v>
-      </c>
-      <c r="I55" t="s">
-        <v>264</v>
-      </c>
-      <c r="J55" t="str">
-        <f t="shared" si="6"/>
-        <v>catalyst</v>
-      </c>
-      <c r="K55" t="s">
-        <v>265</v>
-      </c>
-      <c r="L55" t="str">
+      <c r="H80" t="str">
         <f t="shared" si="8"/>
         <v>ico_catalyst</v>
       </c>
-      <c r="M55" t="s">
+      <c r="I80" t="s">
+        <v>264</v>
+      </c>
+      <c r="L80" t="str">
+        <f t="shared" si="7"/>
+        <v>catalyst</v>
+      </c>
+      <c r="M80" t="s">
+        <v>265</v>
+      </c>
+      <c r="N80" t="str">
+        <f t="shared" si="9"/>
+        <v>ico_catalyst</v>
+      </c>
+      <c r="O80" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
-      <c r="M60" t="s">
+    <row r="85" spans="1:17">
+      <c r="O85" t="s">
         <v>279</v>
       </c>
-      <c r="N60" t="s">
+      <c r="P85" t="s">
         <v>280</v>
       </c>
-      <c r="O60" t="s">
+      <c r="Q85" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
-      <c r="A61" s="17" t="s">
+    <row r="86" spans="1:17">
+      <c r="A86" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B86" t="s">
         <v>274</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C86" t="s">
         <v>283</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D86" t="s">
         <v>274</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E86" t="s">
         <v>284</v>
       </c>
-      <c r="G61" s="17" t="s">
+      <c r="G86" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H86" t="s">
         <v>286</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I86" t="s">
         <v>287</v>
       </c>
-      <c r="J61" t="s">
+      <c r="L86" t="s">
         <v>286</v>
       </c>
-      <c r="K61" t="s">
+      <c r="M86" t="s">
         <v>288</v>
       </c>
-      <c r="M61" t="s">
+      <c r="O86" t="s">
         <v>289</v>
       </c>
-      <c r="N61" t="s">
+      <c r="P86" t="s">
         <v>290</v>
       </c>
-      <c r="O61" t="s">
+      <c r="Q86" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
-      <c r="A62" s="17" t="s">
+    <row r="87" spans="1:17">
+      <c r="A87" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B87" t="s">
         <v>275</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C87" t="s">
         <v>283</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D87" t="s">
         <v>275</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E87" t="s">
         <v>284</v>
       </c>
-      <c r="G62" s="17" t="s">
+      <c r="G87" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H87" t="s">
         <v>292</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I87" t="s">
         <v>287</v>
       </c>
-      <c r="J62" t="s">
+      <c r="L87" t="s">
         <v>292</v>
       </c>
-      <c r="K62" t="s">
+      <c r="M87" t="s">
         <v>288</v>
       </c>
-      <c r="M62" t="s">
+      <c r="O87" t="s">
         <v>293</v>
       </c>
-      <c r="N62" t="s">
+      <c r="P87" t="s">
         <v>294</v>
       </c>
-      <c r="O62" t="s">
+      <c r="Q87" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
-      <c r="A63" s="17" t="s">
+    <row r="88" spans="1:17">
+      <c r="A88" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B88" t="s">
         <v>276</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C88" t="s">
         <v>283</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D88" t="s">
         <v>276</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E88" t="s">
         <v>284</v>
       </c>
-      <c r="G63" s="17" t="s">
+      <c r="G88" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H88" t="s">
         <v>296</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I88" t="s">
         <v>287</v>
       </c>
-      <c r="J63" t="s">
+      <c r="L88" t="s">
         <v>296</v>
       </c>
-      <c r="K63" t="s">
+      <c r="M88" t="s">
         <v>288</v>
       </c>
-      <c r="M63" t="s">
+      <c r="O88" t="s">
         <v>297</v>
       </c>
-      <c r="N63" t="s">
+      <c r="P88" t="s">
         <v>298</v>
       </c>
-      <c r="O63" t="s">
+      <c r="Q88" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
-      <c r="A64" s="17" t="s">
+    <row r="89" spans="1:17">
+      <c r="A89" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B89" t="s">
         <v>277</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C89" t="s">
         <v>283</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D89" t="s">
         <v>277</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E89" t="s">
         <v>284</v>
       </c>
-      <c r="G64" s="17" t="s">
+      <c r="G89" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H89" t="s">
         <v>300</v>
       </c>
-      <c r="I64" t="s">
+      <c r="I89" t="s">
         <v>287</v>
       </c>
-      <c r="J64" t="s">
+      <c r="L89" t="s">
         <v>300</v>
       </c>
-      <c r="K64" t="s">
+      <c r="M89" t="s">
         <v>288</v>
       </c>
-      <c r="M64" t="s">
+      <c r="O89" t="s">
         <v>301</v>
       </c>
-      <c r="N64" t="s">
+      <c r="P89" t="s">
         <v>302</v>
       </c>
-      <c r="O64" t="s">
+      <c r="Q89" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
-      <c r="A65" s="17" t="s">
+    <row r="90" spans="1:17">
+      <c r="A90" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B90" t="s">
         <v>278</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C90" t="s">
         <v>283</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D90" t="s">
         <v>278</v>
       </c>
-      <c r="G65" s="17" t="s">
+      <c r="G90" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H90" t="s">
         <v>304</v>
       </c>
-      <c r="I65" t="s">
+      <c r="I90" t="s">
         <v>287</v>
       </c>
-      <c r="J65" t="s">
+      <c r="L90" t="s">
         <v>304</v>
       </c>
-      <c r="K65" t="s">
+      <c r="M90" t="s">
         <v>288</v>
       </c>
-      <c r="M65" t="s">
+      <c r="O90" t="s">
         <v>305</v>
       </c>
-      <c r="N65" t="s">
+      <c r="P90" t="s">
         <v>306</v>
       </c>
-      <c r="O65" t="s">
+      <c r="Q90" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
-      <c r="A66" s="17"/>
-      <c r="G66" s="17" t="s">
+    <row r="91" spans="1:17">
+      <c r="A91" s="17"/>
+      <c r="G91" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H91" t="s">
         <v>308</v>
       </c>
-      <c r="I66" t="s">
+      <c r="I91" t="s">
         <v>287</v>
       </c>
-      <c r="J66" t="s">
+      <c r="L91" t="s">
         <v>308</v>
       </c>
-      <c r="K66" t="s">
+      <c r="M91" t="s">
         <v>288</v>
       </c>
-      <c r="M66" t="s">
+      <c r="O91" t="s">
         <v>309</v>
       </c>
-      <c r="N66" t="s">
+      <c r="P91" t="s">
         <v>310</v>
       </c>
-      <c r="O66" t="s">
+      <c r="Q91" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
-      <c r="A67" s="17"/>
-      <c r="G67" s="17" t="s">
+    <row r="92" spans="1:17">
+      <c r="A92" s="17"/>
+      <c r="G92" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H92" t="s">
         <v>312</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I92" t="s">
         <v>287</v>
       </c>
-      <c r="J67" t="s">
+      <c r="L92" t="s">
         <v>312</v>
       </c>
-      <c r="K67" t="s">
+      <c r="M92" t="s">
         <v>288</v>
       </c>
-      <c r="M67" t="s">
+      <c r="O92" t="s">
         <v>313</v>
       </c>
-      <c r="N67" t="s">
+      <c r="P92" t="s">
         <v>314</v>
       </c>
-      <c r="O67" t="s">
+      <c r="Q92" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
-      <c r="G68" s="17" t="s">
+    <row r="93" spans="1:17">
+      <c r="G93" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H93" t="s">
         <v>316</v>
       </c>
-      <c r="I68" t="s">
+      <c r="I93" t="s">
         <v>287</v>
       </c>
-      <c r="J68" t="s">
+      <c r="L93" t="s">
         <v>316</v>
       </c>
-      <c r="K68" t="s">
+      <c r="M93" t="s">
         <v>288</v>
       </c>
-      <c r="M68" t="s">
+      <c r="O93" t="s">
         <v>317</v>
       </c>
-      <c r="N68" t="s">
+      <c r="P93" t="s">
         <v>318</v>
       </c>
-      <c r="O68" t="s">
+      <c r="Q93" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
-      <c r="G69" s="17" t="s">
+    <row r="94" spans="1:17">
+      <c r="G94" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H94" t="s">
         <v>320</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I94" t="s">
         <v>287</v>
       </c>
-      <c r="J69" t="s">
+      <c r="L94" t="s">
         <v>320</v>
       </c>
-      <c r="K69" t="s">
+      <c r="M94" t="s">
         <v>288</v>
       </c>
-      <c r="M69" t="s">
+      <c r="O94" t="s">
         <v>321</v>
       </c>
-      <c r="N69" t="s">
+      <c r="P94" t="s">
         <v>322</v>
       </c>
-      <c r="O69" t="s">
+      <c r="Q94" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
-      <c r="G70" s="17" t="s">
+    <row r="95" spans="1:17">
+      <c r="G95" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H95" t="s">
         <v>324</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I95" t="s">
         <v>287</v>
       </c>
-      <c r="J70" t="s">
+      <c r="L95" t="s">
         <v>324</v>
       </c>
-      <c r="K70" t="s">
+      <c r="M95" t="s">
         <v>288</v>
       </c>
-      <c r="M70" t="s">
+      <c r="O95" t="s">
         <v>325</v>
       </c>
-      <c r="N70" t="s">
+      <c r="P95" t="s">
         <v>326</v>
       </c>
-      <c r="O70" t="s">
+      <c r="Q95" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
-      <c r="G71" s="17" t="s">
+    <row r="96" spans="1:17">
+      <c r="G96" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H96" t="s">
         <v>328</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I96" t="s">
         <v>287</v>
       </c>
-      <c r="J71" t="s">
+      <c r="L96" t="s">
         <v>328</v>
       </c>
-      <c r="K71" t="s">
+      <c r="M96" t="s">
         <v>288</v>
       </c>
-      <c r="M71" t="s">
+      <c r="O96" t="s">
         <v>329</v>
       </c>
-      <c r="N71" t="s">
+      <c r="P96" t="s">
         <v>330</v>
       </c>
-      <c r="O71" t="s">
+      <c r="Q96" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
-      <c r="G72" s="17" t="s">
+    <row r="97" spans="1:13">
+      <c r="G97" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H97" t="s">
         <v>332</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I97" t="s">
         <v>287</v>
       </c>
-      <c r="J72" t="s">
+      <c r="L97" t="s">
         <v>332</v>
       </c>
-      <c r="K72" t="s">
+      <c r="M97" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
-      <c r="A76" t="s">
+    <row r="101" spans="1:13">
+      <c r="A101" t="s">
         <v>260</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B101" t="s">
         <v>333</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C101" t="s">
         <v>334</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D101" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
-      <c r="A77" t="s">
+    <row r="102" spans="1:13">
+      <c r="A102" t="s">
         <v>267</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B102" t="s">
         <v>333</v>
       </c>
-      <c r="C77" t="str">
-        <f>"show_"&amp;A77</f>
+      <c r="C102" t="str">
+        <f>"show_"&amp;A102</f>
         <v>show_hydro</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D102" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
-      <c r="A78" t="s">
+    <row r="103" spans="1:13">
+      <c r="A103" t="s">
         <v>268</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B103" t="s">
         <v>333</v>
       </c>
-      <c r="C78" t="str">
-        <f t="shared" ref="C78:C87" si="9">"show_"&amp;A78</f>
+      <c r="C103" t="str">
+        <f t="shared" ref="C103:C112" si="10">"show_"&amp;A103</f>
         <v>show_anemo</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D103" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
-      <c r="A79" t="s">
+    <row r="104" spans="1:13">
+      <c r="A104" t="s">
         <v>269</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B104" t="s">
         <v>333</v>
       </c>
-      <c r="C79" t="str">
-        <f t="shared" si="9"/>
+      <c r="C104" t="str">
+        <f t="shared" si="10"/>
         <v>show_electro</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D104" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
-      <c r="A80" t="s">
+    <row r="105" spans="1:13">
+      <c r="A105" t="s">
         <v>270</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B105" t="s">
         <v>333</v>
       </c>
-      <c r="C80" t="str">
-        <f t="shared" si="9"/>
+      <c r="C105" t="str">
+        <f t="shared" si="10"/>
         <v>show_dendor</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D105" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
-      <c r="A81" t="s">
+    <row r="106" spans="1:13">
+      <c r="A106" t="s">
         <v>271</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B106" t="s">
         <v>333</v>
       </c>
-      <c r="C81" t="str">
-        <f t="shared" si="9"/>
+      <c r="C106" t="str">
+        <f t="shared" si="10"/>
         <v>show_cryo</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D106" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
-      <c r="A82" t="s">
+    <row r="107" spans="1:13">
+      <c r="A107" t="s">
         <v>272</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B107" t="s">
         <v>333</v>
       </c>
-      <c r="C82" t="str">
-        <f t="shared" si="9"/>
+      <c r="C107" t="str">
+        <f t="shared" si="10"/>
         <v>show_geo</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D107" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
-      <c r="A83" t="s">
+    <row r="108" spans="1:13">
+      <c r="A108" t="s">
         <v>274</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B108" t="s">
         <v>333</v>
       </c>
-      <c r="C83" t="str">
-        <f t="shared" si="9"/>
+      <c r="C108" t="str">
+        <f t="shared" si="10"/>
         <v>show_sword</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D108" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="A84" t="s">
+    <row r="109" spans="1:13">
+      <c r="A109" t="s">
         <v>275</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B109" t="s">
         <v>333</v>
       </c>
-      <c r="C84" t="str">
-        <f t="shared" si="9"/>
+      <c r="C109" t="str">
+        <f t="shared" si="10"/>
         <v>show_claymore</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D109" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85" t="s">
+    <row r="110" spans="1:13">
+      <c r="A110" t="s">
         <v>276</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B110" t="s">
         <v>333</v>
       </c>
-      <c r="C85" t="str">
-        <f t="shared" si="9"/>
+      <c r="C110" t="str">
+        <f t="shared" si="10"/>
         <v>show_polearm</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D110" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86" t="s">
+    <row r="111" spans="1:13">
+      <c r="A111" t="s">
         <v>277</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B111" t="s">
         <v>333</v>
       </c>
-      <c r="C86" t="str">
-        <f t="shared" si="9"/>
+      <c r="C111" t="str">
+        <f t="shared" si="10"/>
         <v>show_bow</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D111" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" t="s">
+    <row r="112" spans="1:13">
+      <c r="A112" t="s">
         <v>278</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B112" t="s">
         <v>333</v>
       </c>
-      <c r="C87" t="str">
-        <f t="shared" si="9"/>
+      <c r="C112" t="str">
+        <f t="shared" si="10"/>
         <v>show_catalyst</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D112" t="s">
         <v>335</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Characters IMG CHANGED & RECREATED
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vocaloid2048\Desktop\File\App\GenshinHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1397E02B-ED08-41BE-87CE-1139CEE861B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A856BDE-8020-44E6-9C40-101C09375CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{DB4DA38A-4327-40F6-9D21-54F6AE12F3DD}"/>
+    <workbookView xWindow="30360" yWindow="690" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{DB4DA38A-4327-40F6-9D21-54F6AE12F3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Home_List" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2233" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="508">
   <si>
     <t>"&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1903,6 +1903,242 @@
   <si>
     <t>//Add at 210820</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REN "</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character_Albedo_Portrait.png</t>
+  </si>
+  <si>
+    <t>" "</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Albedo.png</t>
+  </si>
+  <si>
+    <t>Character_Amber_Portrait.png</t>
+  </si>
+  <si>
+    <t>Amber.png</t>
+  </si>
+  <si>
+    <t>Character_Barbara_Portrait.png</t>
+  </si>
+  <si>
+    <t>Barbara.png</t>
+  </si>
+  <si>
+    <t>Character_Beidou_Portrait.png</t>
+  </si>
+  <si>
+    <t>Beidou.png</t>
+  </si>
+  <si>
+    <t>Character_Bennett_Portrait.png</t>
+  </si>
+  <si>
+    <t>Bennett.png</t>
+  </si>
+  <si>
+    <t>Character_Chongyun_Portrait.png</t>
+  </si>
+  <si>
+    <t>Chongyun.png</t>
+  </si>
+  <si>
+    <t>Character_Diluc_Portrait.png</t>
+  </si>
+  <si>
+    <t>Diluc.png</t>
+  </si>
+  <si>
+    <t>Character_Diona_Portrait.png</t>
+  </si>
+  <si>
+    <t>Diona.png</t>
+  </si>
+  <si>
+    <t>Character_Fischl_Portrait.png</t>
+  </si>
+  <si>
+    <t>Fischl.png</t>
+  </si>
+  <si>
+    <t>Character_Ganyu_Portrait.png</t>
+  </si>
+  <si>
+    <t>Ganyu.png</t>
+  </si>
+  <si>
+    <t>Character_Hu_Tao_Portrait.png</t>
+  </si>
+  <si>
+    <t>Hu_Tao.png</t>
+  </si>
+  <si>
+    <t>Character_Jean_Portrait.png</t>
+  </si>
+  <si>
+    <t>Jean.png</t>
+  </si>
+  <si>
+    <t>Character_Kaedehara_Kazuha_Portrait.png</t>
+  </si>
+  <si>
+    <t>Kaedehara_Kazuha.png</t>
+  </si>
+  <si>
+    <t>Character_Kaeya_Portrait.png</t>
+  </si>
+  <si>
+    <t>Kaeya.png</t>
+  </si>
+  <si>
+    <t>Character_Kamisato_Ayaka_Portrait.png</t>
+  </si>
+  <si>
+    <t>Kamisato_Ayaka.png</t>
+  </si>
+  <si>
+    <t>Character_Keqing_Portrait.png</t>
+  </si>
+  <si>
+    <t>Keqing.png</t>
+  </si>
+  <si>
+    <t>Character_Klee_Portrait.png</t>
+  </si>
+  <si>
+    <t>Klee.png</t>
+  </si>
+  <si>
+    <t>Character_Kujou_Sara_Portrait.webp</t>
+  </si>
+  <si>
+    <t>Kujou_Sara.webp</t>
+  </si>
+  <si>
+    <t>Character_Lisa_Portrait.png</t>
+  </si>
+  <si>
+    <t>Lisa.png</t>
+  </si>
+  <si>
+    <t>Character_Mona_Portrait.png</t>
+  </si>
+  <si>
+    <t>Mona.png</t>
+  </si>
+  <si>
+    <t>Character_Ningguang_Portrait.png</t>
+  </si>
+  <si>
+    <t>Ningguang.png</t>
+  </si>
+  <si>
+    <t>Character_Noelle_Portrait.png</t>
+  </si>
+  <si>
+    <t>Noelle.png</t>
+  </si>
+  <si>
+    <t>Character_Qiqi_Portrait.png</t>
+  </si>
+  <si>
+    <t>Qiqi.png</t>
+  </si>
+  <si>
+    <t>Character_Raiden_Shogun_Portrait .png</t>
+  </si>
+  <si>
+    <t>Raiden_Shogun .png</t>
+  </si>
+  <si>
+    <t>Character_Razor_Portrait.png</t>
+  </si>
+  <si>
+    <t>Razor.png</t>
+  </si>
+  <si>
+    <t>Character_Rosaria_Portrait.png</t>
+  </si>
+  <si>
+    <t>Rosaria.png</t>
+  </si>
+  <si>
+    <t>Character_Sangonomiya_Kokomi_Portrait.webp</t>
+  </si>
+  <si>
+    <t>Sangonomiya_Kokomi.webp</t>
+  </si>
+  <si>
+    <t>Character_Sayu_Portrait.png</t>
+  </si>
+  <si>
+    <t>Sayu.png</t>
+  </si>
+  <si>
+    <t>Character_Sucrose_Portrait.png</t>
+  </si>
+  <si>
+    <t>Sucrose.png</t>
+  </si>
+  <si>
+    <t>Character_Tartaglia_Portrait.png</t>
+  </si>
+  <si>
+    <t>Tartaglia.png</t>
+  </si>
+  <si>
+    <t>Character_Venti_Portrait.png</t>
+  </si>
+  <si>
+    <t>Venti.png</t>
+  </si>
+  <si>
+    <t>Character_Xiangling_Portrait.png</t>
+  </si>
+  <si>
+    <t>Xiangling.png</t>
+  </si>
+  <si>
+    <t>Character_Xiao_Portrait.png</t>
+  </si>
+  <si>
+    <t>Xiao.png</t>
+  </si>
+  <si>
+    <t>Character_Xingqiu_Portrait.png</t>
+  </si>
+  <si>
+    <t>Xingqiu.png</t>
+  </si>
+  <si>
+    <t>Character_Xinyan_Portrait.png</t>
+  </si>
+  <si>
+    <t>Xinyan.png</t>
+  </si>
+  <si>
+    <t>Character_Yanfei_Portrait.png</t>
+  </si>
+  <si>
+    <t>Yanfei.png</t>
+  </si>
+  <si>
+    <t>Character_Yoimiya_Portrait.png</t>
+  </si>
+  <si>
+    <t>Yoimiya.png</t>
+  </si>
+  <si>
+    <t>Character_Zhongli_Portrait.png</t>
+  </si>
+  <si>
+    <t>Zhongli.png</t>
   </si>
 </sst>
 </file>
@@ -7935,10 +8171,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C5A84A-5C7F-451F-A1D8-4D9A74023F1A}">
-  <dimension ref="A1:Y112"/>
+  <dimension ref="A1:Y152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115:I152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -11662,6 +11898,804 @@
       </c>
       <c r="D112" t="s">
         <v>335</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" t="s">
+        <v>430</v>
+      </c>
+      <c r="B115" t="s">
+        <v>431</v>
+      </c>
+      <c r="C115" t="s">
+        <v>432</v>
+      </c>
+      <c r="D115" t="str">
+        <f>LOWER(H115)</f>
+        <v>albedo.png</v>
+      </c>
+      <c r="E115" t="s">
+        <v>349</v>
+      </c>
+      <c r="H115" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" t="s">
+        <v>430</v>
+      </c>
+      <c r="B116" t="s">
+        <v>434</v>
+      </c>
+      <c r="C116" t="s">
+        <v>432</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" ref="D116:D152" si="11">LOWER(H116)</f>
+        <v>amber.png</v>
+      </c>
+      <c r="E116" t="s">
+        <v>349</v>
+      </c>
+      <c r="H116" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" t="s">
+        <v>430</v>
+      </c>
+      <c r="B117" t="s">
+        <v>436</v>
+      </c>
+      <c r="C117" t="s">
+        <v>432</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="11"/>
+        <v>barbara.png</v>
+      </c>
+      <c r="E117" t="s">
+        <v>349</v>
+      </c>
+      <c r="H117" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" t="s">
+        <v>430</v>
+      </c>
+      <c r="B118" t="s">
+        <v>438</v>
+      </c>
+      <c r="C118" t="s">
+        <v>432</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" si="11"/>
+        <v>beidou.png</v>
+      </c>
+      <c r="E118" t="s">
+        <v>349</v>
+      </c>
+      <c r="H118" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" t="s">
+        <v>430</v>
+      </c>
+      <c r="B119" t="s">
+        <v>440</v>
+      </c>
+      <c r="C119" t="s">
+        <v>432</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="11"/>
+        <v>bennett.png</v>
+      </c>
+      <c r="E119" t="s">
+        <v>349</v>
+      </c>
+      <c r="H119" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" t="s">
+        <v>430</v>
+      </c>
+      <c r="B120" t="s">
+        <v>442</v>
+      </c>
+      <c r="C120" t="s">
+        <v>432</v>
+      </c>
+      <c r="D120" t="str">
+        <f t="shared" si="11"/>
+        <v>chongyun.png</v>
+      </c>
+      <c r="E120" t="s">
+        <v>349</v>
+      </c>
+      <c r="H120" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" t="s">
+        <v>430</v>
+      </c>
+      <c r="B121" t="s">
+        <v>444</v>
+      </c>
+      <c r="C121" t="s">
+        <v>432</v>
+      </c>
+      <c r="D121" t="str">
+        <f t="shared" si="11"/>
+        <v>diluc.png</v>
+      </c>
+      <c r="E121" t="s">
+        <v>349</v>
+      </c>
+      <c r="H121" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" t="s">
+        <v>430</v>
+      </c>
+      <c r="B122" t="s">
+        <v>446</v>
+      </c>
+      <c r="C122" t="s">
+        <v>432</v>
+      </c>
+      <c r="D122" t="str">
+        <f t="shared" si="11"/>
+        <v>diona.png</v>
+      </c>
+      <c r="E122" t="s">
+        <v>349</v>
+      </c>
+      <c r="H122" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" t="s">
+        <v>430</v>
+      </c>
+      <c r="B123" t="s">
+        <v>448</v>
+      </c>
+      <c r="C123" t="s">
+        <v>432</v>
+      </c>
+      <c r="D123" t="str">
+        <f t="shared" si="11"/>
+        <v>fischl.png</v>
+      </c>
+      <c r="E123" t="s">
+        <v>349</v>
+      </c>
+      <c r="H123" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" t="s">
+        <v>430</v>
+      </c>
+      <c r="B124" t="s">
+        <v>450</v>
+      </c>
+      <c r="C124" t="s">
+        <v>432</v>
+      </c>
+      <c r="D124" t="str">
+        <f t="shared" si="11"/>
+        <v>ganyu.png</v>
+      </c>
+      <c r="E124" t="s">
+        <v>349</v>
+      </c>
+      <c r="H124" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" t="s">
+        <v>430</v>
+      </c>
+      <c r="B125" t="s">
+        <v>452</v>
+      </c>
+      <c r="C125" t="s">
+        <v>432</v>
+      </c>
+      <c r="D125" t="str">
+        <f t="shared" si="11"/>
+        <v>hu_tao.png</v>
+      </c>
+      <c r="E125" t="s">
+        <v>349</v>
+      </c>
+      <c r="H125" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" t="s">
+        <v>430</v>
+      </c>
+      <c r="B126" t="s">
+        <v>454</v>
+      </c>
+      <c r="C126" t="s">
+        <v>432</v>
+      </c>
+      <c r="D126" t="str">
+        <f t="shared" si="11"/>
+        <v>jean.png</v>
+      </c>
+      <c r="E126" t="s">
+        <v>349</v>
+      </c>
+      <c r="H126" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" t="s">
+        <v>430</v>
+      </c>
+      <c r="B127" t="s">
+        <v>456</v>
+      </c>
+      <c r="C127" t="s">
+        <v>432</v>
+      </c>
+      <c r="D127" t="str">
+        <f t="shared" si="11"/>
+        <v>kaedehara_kazuha.png</v>
+      </c>
+      <c r="E127" t="s">
+        <v>349</v>
+      </c>
+      <c r="H127" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" t="s">
+        <v>430</v>
+      </c>
+      <c r="B128" t="s">
+        <v>458</v>
+      </c>
+      <c r="C128" t="s">
+        <v>432</v>
+      </c>
+      <c r="D128" t="str">
+        <f t="shared" si="11"/>
+        <v>kaeya.png</v>
+      </c>
+      <c r="E128" t="s">
+        <v>349</v>
+      </c>
+      <c r="H128" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129" t="s">
+        <v>430</v>
+      </c>
+      <c r="B129" t="s">
+        <v>460</v>
+      </c>
+      <c r="C129" t="s">
+        <v>432</v>
+      </c>
+      <c r="D129" t="str">
+        <f t="shared" si="11"/>
+        <v>kamisato_ayaka.png</v>
+      </c>
+      <c r="E129" t="s">
+        <v>349</v>
+      </c>
+      <c r="H129" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130" t="s">
+        <v>430</v>
+      </c>
+      <c r="B130" t="s">
+        <v>462</v>
+      </c>
+      <c r="C130" t="s">
+        <v>432</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" si="11"/>
+        <v>keqing.png</v>
+      </c>
+      <c r="E130" t="s">
+        <v>349</v>
+      </c>
+      <c r="H130" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131" t="s">
+        <v>430</v>
+      </c>
+      <c r="B131" t="s">
+        <v>464</v>
+      </c>
+      <c r="C131" t="s">
+        <v>432</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" si="11"/>
+        <v>klee.png</v>
+      </c>
+      <c r="E131" t="s">
+        <v>349</v>
+      </c>
+      <c r="H131" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" t="s">
+        <v>430</v>
+      </c>
+      <c r="B132" t="s">
+        <v>466</v>
+      </c>
+      <c r="C132" t="s">
+        <v>432</v>
+      </c>
+      <c r="D132" t="str">
+        <f t="shared" si="11"/>
+        <v>kujou_sara.webp</v>
+      </c>
+      <c r="E132" t="s">
+        <v>349</v>
+      </c>
+      <c r="H132" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" t="s">
+        <v>430</v>
+      </c>
+      <c r="B133" t="s">
+        <v>468</v>
+      </c>
+      <c r="C133" t="s">
+        <v>432</v>
+      </c>
+      <c r="D133" t="str">
+        <f t="shared" si="11"/>
+        <v>lisa.png</v>
+      </c>
+      <c r="E133" t="s">
+        <v>349</v>
+      </c>
+      <c r="H133" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" t="s">
+        <v>430</v>
+      </c>
+      <c r="B134" t="s">
+        <v>470</v>
+      </c>
+      <c r="C134" t="s">
+        <v>432</v>
+      </c>
+      <c r="D134" t="str">
+        <f t="shared" si="11"/>
+        <v>mona.png</v>
+      </c>
+      <c r="E134" t="s">
+        <v>349</v>
+      </c>
+      <c r="H134" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" t="s">
+        <v>430</v>
+      </c>
+      <c r="B135" t="s">
+        <v>472</v>
+      </c>
+      <c r="C135" t="s">
+        <v>432</v>
+      </c>
+      <c r="D135" t="str">
+        <f t="shared" si="11"/>
+        <v>ningguang.png</v>
+      </c>
+      <c r="E135" t="s">
+        <v>349</v>
+      </c>
+      <c r="H135" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" t="s">
+        <v>430</v>
+      </c>
+      <c r="B136" t="s">
+        <v>474</v>
+      </c>
+      <c r="C136" t="s">
+        <v>432</v>
+      </c>
+      <c r="D136" t="str">
+        <f t="shared" si="11"/>
+        <v>noelle.png</v>
+      </c>
+      <c r="E136" t="s">
+        <v>349</v>
+      </c>
+      <c r="H136" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137" t="s">
+        <v>430</v>
+      </c>
+      <c r="B137" t="s">
+        <v>476</v>
+      </c>
+      <c r="C137" t="s">
+        <v>432</v>
+      </c>
+      <c r="D137" t="str">
+        <f t="shared" si="11"/>
+        <v>qiqi.png</v>
+      </c>
+      <c r="E137" t="s">
+        <v>349</v>
+      </c>
+      <c r="H137" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" t="s">
+        <v>430</v>
+      </c>
+      <c r="B138" t="s">
+        <v>478</v>
+      </c>
+      <c r="C138" t="s">
+        <v>432</v>
+      </c>
+      <c r="D138" t="str">
+        <f t="shared" si="11"/>
+        <v>raiden_shogun .png</v>
+      </c>
+      <c r="E138" t="s">
+        <v>349</v>
+      </c>
+      <c r="H138" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
+      <c r="A139" t="s">
+        <v>430</v>
+      </c>
+      <c r="B139" t="s">
+        <v>480</v>
+      </c>
+      <c r="C139" t="s">
+        <v>432</v>
+      </c>
+      <c r="D139" t="str">
+        <f t="shared" si="11"/>
+        <v>razor.png</v>
+      </c>
+      <c r="E139" t="s">
+        <v>349</v>
+      </c>
+      <c r="H139" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
+      <c r="A140" t="s">
+        <v>430</v>
+      </c>
+      <c r="B140" t="s">
+        <v>482</v>
+      </c>
+      <c r="C140" t="s">
+        <v>432</v>
+      </c>
+      <c r="D140" t="str">
+        <f t="shared" si="11"/>
+        <v>rosaria.png</v>
+      </c>
+      <c r="E140" t="s">
+        <v>349</v>
+      </c>
+      <c r="H140" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
+      <c r="A141" t="s">
+        <v>430</v>
+      </c>
+      <c r="B141" t="s">
+        <v>484</v>
+      </c>
+      <c r="C141" t="s">
+        <v>432</v>
+      </c>
+      <c r="D141" t="str">
+        <f t="shared" si="11"/>
+        <v>sangonomiya_kokomi.webp</v>
+      </c>
+      <c r="E141" t="s">
+        <v>349</v>
+      </c>
+      <c r="H141" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
+      <c r="A142" t="s">
+        <v>430</v>
+      </c>
+      <c r="B142" t="s">
+        <v>486</v>
+      </c>
+      <c r="C142" t="s">
+        <v>432</v>
+      </c>
+      <c r="D142" t="str">
+        <f t="shared" si="11"/>
+        <v>sayu.png</v>
+      </c>
+      <c r="E142" t="s">
+        <v>349</v>
+      </c>
+      <c r="H142" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
+      <c r="A143" t="s">
+        <v>430</v>
+      </c>
+      <c r="B143" t="s">
+        <v>488</v>
+      </c>
+      <c r="C143" t="s">
+        <v>432</v>
+      </c>
+      <c r="D143" t="str">
+        <f t="shared" si="11"/>
+        <v>sucrose.png</v>
+      </c>
+      <c r="E143" t="s">
+        <v>349</v>
+      </c>
+      <c r="H143" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144" t="s">
+        <v>430</v>
+      </c>
+      <c r="B144" t="s">
+        <v>490</v>
+      </c>
+      <c r="C144" t="s">
+        <v>432</v>
+      </c>
+      <c r="D144" t="str">
+        <f t="shared" si="11"/>
+        <v>tartaglia.png</v>
+      </c>
+      <c r="E144" t="s">
+        <v>349</v>
+      </c>
+      <c r="H144" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8">
+      <c r="A145" t="s">
+        <v>430</v>
+      </c>
+      <c r="B145" t="s">
+        <v>492</v>
+      </c>
+      <c r="C145" t="s">
+        <v>432</v>
+      </c>
+      <c r="D145" t="str">
+        <f t="shared" si="11"/>
+        <v>venti.png</v>
+      </c>
+      <c r="E145" t="s">
+        <v>349</v>
+      </c>
+      <c r="H145" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
+      <c r="A146" t="s">
+        <v>430</v>
+      </c>
+      <c r="B146" t="s">
+        <v>494</v>
+      </c>
+      <c r="C146" t="s">
+        <v>432</v>
+      </c>
+      <c r="D146" t="str">
+        <f t="shared" si="11"/>
+        <v>xiangling.png</v>
+      </c>
+      <c r="E146" t="s">
+        <v>349</v>
+      </c>
+      <c r="H146" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8">
+      <c r="A147" t="s">
+        <v>430</v>
+      </c>
+      <c r="B147" t="s">
+        <v>496</v>
+      </c>
+      <c r="C147" t="s">
+        <v>432</v>
+      </c>
+      <c r="D147" t="str">
+        <f t="shared" si="11"/>
+        <v>xiao.png</v>
+      </c>
+      <c r="E147" t="s">
+        <v>349</v>
+      </c>
+      <c r="H147" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
+      <c r="A148" t="s">
+        <v>430</v>
+      </c>
+      <c r="B148" t="s">
+        <v>498</v>
+      </c>
+      <c r="C148" t="s">
+        <v>432</v>
+      </c>
+      <c r="D148" t="str">
+        <f t="shared" si="11"/>
+        <v>xingqiu.png</v>
+      </c>
+      <c r="E148" t="s">
+        <v>349</v>
+      </c>
+      <c r="H148" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149" t="s">
+        <v>430</v>
+      </c>
+      <c r="B149" t="s">
+        <v>500</v>
+      </c>
+      <c r="C149" t="s">
+        <v>432</v>
+      </c>
+      <c r="D149" t="str">
+        <f t="shared" si="11"/>
+        <v>xinyan.png</v>
+      </c>
+      <c r="E149" t="s">
+        <v>349</v>
+      </c>
+      <c r="H149" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150" t="s">
+        <v>430</v>
+      </c>
+      <c r="B150" t="s">
+        <v>502</v>
+      </c>
+      <c r="C150" t="s">
+        <v>432</v>
+      </c>
+      <c r="D150" t="str">
+        <f t="shared" si="11"/>
+        <v>yanfei.png</v>
+      </c>
+      <c r="E150" t="s">
+        <v>349</v>
+      </c>
+      <c r="H150" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151" t="s">
+        <v>430</v>
+      </c>
+      <c r="B151" t="s">
+        <v>504</v>
+      </c>
+      <c r="C151" t="s">
+        <v>432</v>
+      </c>
+      <c r="D151" t="str">
+        <f t="shared" si="11"/>
+        <v>yoimiya.png</v>
+      </c>
+      <c r="E151" t="s">
+        <v>349</v>
+      </c>
+      <c r="H151" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152" t="s">
+        <v>430</v>
+      </c>
+      <c r="B152" t="s">
+        <v>506</v>
+      </c>
+      <c r="C152" t="s">
+        <v>432</v>
+      </c>
+      <c r="D152" t="str">
+        <f t="shared" si="11"/>
+        <v>zhongli.png</v>
+      </c>
+      <c r="E152" t="s">
+        <v>349</v>
+      </c>
+      <c r="H152" t="s">
+        <v>507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weapon Sword, Claymore, Polearm info added
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vocaloid2048\Desktop\File\App\GenshinHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75423AA1-DFDE-45CC-A3BF-85FC4EE715FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74B4381-647E-4A7C-B6F4-7757964BDCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{DB4DA38A-4327-40F6-9D21-54F6AE12F3DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="3" activeTab="6" xr2:uid="{DB4DA38A-4327-40F6-9D21-54F6AE12F3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Home_List" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="工作表1" sheetId="5" r:id="rId4"/>
     <sheet name="klee_CharStatus" sheetId="4" r:id="rId5"/>
     <sheet name="CharEXP" sheetId="6" r:id="rId6"/>
+    <sheet name="WeaponList" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CharEXP!$S$51:$S$91</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6308" uniqueCount="1225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6719" uniqueCount="1541">
   <si>
     <t>"&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4726,12 +4727,1091 @@
     <t>")){return context.getString(R.string.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>ATK</t>
+  </si>
+  <si>
+    <t>ATK%</t>
+  </si>
+  <si>
+    <t>CritDMG%</t>
+  </si>
+  <si>
+    <t>PhyDMG%</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>屬性對照表</t>
+  </si>
+  <si>
+    <t>Meaning'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>元素精通</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>元素充能效率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命值%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻擊力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻擊力%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴擊率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴擊傷害%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴擊傷害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物理傷害%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防禦力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物理傷害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnRech%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>元素充能效率%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EleMas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷刃</t>
+  </si>
+  <si>
+    <t>天目影打刀</t>
+  </si>
+  <si>
+    <t>天空之刃</t>
+  </si>
+  <si>
+    <t>斫峰之刃</t>
+  </si>
+  <si>
+    <t>Sword List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stat_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stat_2</t>
+  </si>
+  <si>
+    <t>zh_hk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zh_cn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ru_ru</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ja_jp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CritRate</t>
+  </si>
+  <si>
+    <t>暴擊率%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防禦力%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEF%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>en_us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>amenoma_kageuchi</t>
+  </si>
+  <si>
+    <t>aquila_favonia</t>
+  </si>
+  <si>
+    <t>blackcliff_longsword</t>
+  </si>
+  <si>
+    <t>cool_steel</t>
+  </si>
+  <si>
+    <t>dark_iron_sword</t>
+  </si>
+  <si>
+    <t>dull_blade</t>
+  </si>
+  <si>
+    <t>favonius_sword</t>
+  </si>
+  <si>
+    <t>festering_desire</t>
+  </si>
+  <si>
+    <t>fillet_blade</t>
+  </si>
+  <si>
+    <t>freedom_sworn</t>
+  </si>
+  <si>
+    <t>harbinger_of_dawn</t>
+  </si>
+  <si>
+    <t>iron_sting</t>
+  </si>
+  <si>
+    <t>lion's_roar</t>
+  </si>
+  <si>
+    <t>mistsplitter_reforged</t>
+  </si>
+  <si>
+    <t>primordial_jade_cutter</t>
+  </si>
+  <si>
+    <t>prototype_rancour</t>
+  </si>
+  <si>
+    <t>royal_longsword</t>
+  </si>
+  <si>
+    <t>sacrificial_sword</t>
+  </si>
+  <si>
+    <t>silver_sword</t>
+  </si>
+  <si>
+    <t>skyrider_sword</t>
+  </si>
+  <si>
+    <t>skyward_blade</t>
+  </si>
+  <si>
+    <t>summit_shaper</t>
+  </si>
+  <si>
+    <t>sword_of_descension</t>
+  </si>
+  <si>
+    <t>the_alley_flash</t>
+  </si>
+  <si>
+    <t>the_black_sword</t>
+  </si>
+  <si>
+    <t>the_flute</t>
+  </si>
+  <si>
+    <t>traveler's_handy_sword</t>
+  </si>
+  <si>
+    <t>Amenoma Kageuchi</t>
+  </si>
+  <si>
+    <t>Aquila Favonia</t>
+  </si>
+  <si>
+    <t>Blackcliff Longsword</t>
+  </si>
+  <si>
+    <t>Cool Steel</t>
+  </si>
+  <si>
+    <t>Dark Iron Sword</t>
+  </si>
+  <si>
+    <t>Dull Blade</t>
+  </si>
+  <si>
+    <t>Favonius Sword</t>
+  </si>
+  <si>
+    <t>Festering Desire</t>
+  </si>
+  <si>
+    <t>Fillet Blade</t>
+  </si>
+  <si>
+    <t>Freedom Sworn</t>
+  </si>
+  <si>
+    <t>Harbinger of Dawn</t>
+  </si>
+  <si>
+    <t>Iron Sting</t>
+  </si>
+  <si>
+    <t>Lion's Roar</t>
+  </si>
+  <si>
+    <t>Mistsplitter Reforged</t>
+  </si>
+  <si>
+    <t>Primordial Jade Cutter</t>
+  </si>
+  <si>
+    <t>Prototype Rancour</t>
+  </si>
+  <si>
+    <t>Royal Longsword</t>
+  </si>
+  <si>
+    <t>Sacrificial Sword</t>
+  </si>
+  <si>
+    <t>Silver Sword</t>
+  </si>
+  <si>
+    <t>Skyrider Sword</t>
+  </si>
+  <si>
+    <t>Skyward Blade</t>
+  </si>
+  <si>
+    <t>Summit Shaper</t>
+  </si>
+  <si>
+    <t>Sword of Descension</t>
+  </si>
+  <si>
+    <t>The Alley Flash</t>
+  </si>
+  <si>
+    <t>The Black Sword</t>
+  </si>
+  <si>
+    <t>The Flute</t>
+  </si>
+  <si>
+    <t>Traveler's Handy Sword</t>
+  </si>
+  <si>
+    <t>Id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATK%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PhyDMG%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CritDMG%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CritRate%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天目影打刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>风鹰剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑岩长剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷刃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗铁剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无锋剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西风剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>腐殖之剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吃虎鱼刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>苍古自由之誓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黎明神剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁蜂刺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>匣里龙吟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雾切之回光</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞天御剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>磐岩结绿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>试作斩岩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宗室长剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>祭礼剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>银剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天空之刃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>斫峰之刃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>降临之剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗巷闪光</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>笛剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>旅行剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>風鷹劍</t>
+  </si>
+  <si>
+    <t>黑岩長劍</t>
+  </si>
+  <si>
+    <t>暗鐵劍</t>
+  </si>
+  <si>
+    <t>無鋒劍</t>
+  </si>
+  <si>
+    <t>西風劍</t>
+  </si>
+  <si>
+    <t>腐殖之劍</t>
+  </si>
+  <si>
+    <t>吃虎魚刀</t>
+  </si>
+  <si>
+    <t>蒼古自由之誓</t>
+  </si>
+  <si>
+    <t>黎明神劍</t>
+  </si>
+  <si>
+    <t>鐵蜂刺</t>
+  </si>
+  <si>
+    <t>匣裡龍吟</t>
+  </si>
+  <si>
+    <t>霧切之迴光</t>
+  </si>
+  <si>
+    <t>磐岩結綠</t>
+  </si>
+  <si>
+    <t>試作斬岩</t>
+  </si>
+  <si>
+    <t>宗室長劍</t>
+  </si>
+  <si>
+    <t>祭禮劍</t>
+  </si>
+  <si>
+    <t>銀劍</t>
+  </si>
+  <si>
+    <t>飛天御劍</t>
+  </si>
+  <si>
+    <t>降臨之劍</t>
+  </si>
+  <si>
+    <t>暗巷閃光</t>
+  </si>
+  <si>
+    <t>黑劍</t>
+  </si>
+  <si>
+    <t>笛劍</t>
+  </si>
+  <si>
+    <t>旅行劍</t>
+  </si>
+  <si>
+    <t>Claymore List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>训练大剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>佣兵重剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以理服人</t>
+  </si>
+  <si>
+    <t>沐浴龙血的剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以理服人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁影阔剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quartz</t>
+  </si>
+  <si>
+    <t>HP%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白铁大剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑岩斩刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西风大剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桂木斩长正</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>千岩古剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>衔珠海皇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>试作古华</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雨裁</t>
+  </si>
+  <si>
+    <t>雨裁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宗室大剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>祭礼大剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>螭骨剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雪葬的星银</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钟剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白影剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天空之傲</t>
+  </si>
+  <si>
+    <t>天空之傲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松籁响起之时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无工之剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狼的末路</t>
+  </si>
+  <si>
+    <t>狼的末路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Waster Greatsword</t>
+  </si>
+  <si>
+    <t>Old Merc's Pal</t>
+  </si>
+  <si>
+    <t>Bloodtainted Greatsword</t>
+  </si>
+  <si>
+    <t>Debate Club</t>
+  </si>
+  <si>
+    <t>Ferrous Shadow</t>
+  </si>
+  <si>
+    <t>Skyrider Greatsword</t>
+  </si>
+  <si>
+    <t>White Iron Greatsword</t>
+  </si>
+  <si>
+    <t>Blackcliff Slasher</t>
+  </si>
+  <si>
+    <t>Favonius Greatsword</t>
+  </si>
+  <si>
+    <t>Katsuragikiri Nagamasa</t>
+  </si>
+  <si>
+    <t>Lithic Blade</t>
+  </si>
+  <si>
+    <t>Luxurious Sea-Lord</t>
+  </si>
+  <si>
+    <t>Prototype Archaic</t>
+  </si>
+  <si>
+    <t>Rainslasher</t>
+  </si>
+  <si>
+    <t>Royal Greatsword</t>
+  </si>
+  <si>
+    <t>Sacrificial Greatsword</t>
+  </si>
+  <si>
+    <t>Serpent Spine</t>
+  </si>
+  <si>
+    <t>Snow-Tombed Starsilver</t>
+  </si>
+  <si>
+    <t>The Bell</t>
+  </si>
+  <si>
+    <t>Whiteblind</t>
+  </si>
+  <si>
+    <t>Skyward Pride</t>
+  </si>
+  <si>
+    <t>Song of Broken Pines</t>
+  </si>
+  <si>
+    <t>The Unforged</t>
+  </si>
+  <si>
+    <t>Wolf's Gravestone</t>
+  </si>
+  <si>
+    <t>waster_greatsword</t>
+  </si>
+  <si>
+    <t>old_merc's_pal</t>
+  </si>
+  <si>
+    <t>bloodtainted_greatsword</t>
+  </si>
+  <si>
+    <t>debate_club</t>
+  </si>
+  <si>
+    <t>quartz</t>
+  </si>
+  <si>
+    <t>ferrous_shadow</t>
+  </si>
+  <si>
+    <t>skyrider_greatsword</t>
+  </si>
+  <si>
+    <t>white_iron_greatsword</t>
+  </si>
+  <si>
+    <t>blackcliff_slasher</t>
+  </si>
+  <si>
+    <t>favonius_greatsword</t>
+  </si>
+  <si>
+    <t>katsuragikiri_nagamasa</t>
+  </si>
+  <si>
+    <t>lithic_blade</t>
+  </si>
+  <si>
+    <t>luxurious_sea-lord</t>
+  </si>
+  <si>
+    <t>prototype_archaic</t>
+  </si>
+  <si>
+    <t>rainslasher</t>
+  </si>
+  <si>
+    <t>royal_greatsword</t>
+  </si>
+  <si>
+    <t>sacrificial_greatsword</t>
+  </si>
+  <si>
+    <t>serpent_spine</t>
+  </si>
+  <si>
+    <t>snow-tombed_starsilver</t>
+  </si>
+  <si>
+    <t>the_bell</t>
+  </si>
+  <si>
+    <t>whiteblind</t>
+  </si>
+  <si>
+    <t>skyward_pride</t>
+  </si>
+  <si>
+    <t>song_of_broken_pines</t>
+  </si>
+  <si>
+    <t>the_unforged</t>
+  </si>
+  <si>
+    <t>wolf's_gravestone</t>
+  </si>
+  <si>
+    <t>訓練大劍</t>
+  </si>
+  <si>
+    <t>傭兵重劍</t>
+  </si>
+  <si>
+    <t>沐浴龍血的劍</t>
+  </si>
+  <si>
+    <t>鐵影闊劍</t>
+  </si>
+  <si>
+    <t>飛天大御劍</t>
+  </si>
+  <si>
+    <t>白鐵大劍</t>
+  </si>
+  <si>
+    <t>黑岩斬刀</t>
+  </si>
+  <si>
+    <t>西風大劍</t>
+  </si>
+  <si>
+    <t>桂木斬長正</t>
+  </si>
+  <si>
+    <t>千巖古劍</t>
+  </si>
+  <si>
+    <t>銜珠海皇</t>
+  </si>
+  <si>
+    <t>試作古華</t>
+  </si>
+  <si>
+    <t>宗室大劍</t>
+  </si>
+  <si>
+    <t>祭禮大劍</t>
+  </si>
+  <si>
+    <t>螭骨劍</t>
+  </si>
+  <si>
+    <t>雪葬的星銀</t>
+  </si>
+  <si>
+    <t>鍾劍</t>
+  </si>
+  <si>
+    <t>白影劍</t>
+  </si>
+  <si>
+    <t>松籟響起之時</t>
+  </si>
+  <si>
+    <t>無工之劍</t>
+  </si>
+  <si>
+    <t>飞天大御剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>石英大剑</t>
+  </si>
+  <si>
+    <t>石英大劍</t>
+  </si>
+  <si>
+    <t>Polearm List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beginner's Protector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新手长枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iron Point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁尖枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>White Tassel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白缨枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑缨枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black Tassel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Halberd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钺矛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crescent Pike</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>流月针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prototype Starglitter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>试作星镰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kitain Cross Spear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>喜多院十文字</t>
+  </si>
+  <si>
+    <t>喜多院十文字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dragonspine Spear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙脊长枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Royal Spear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宗室猎枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Catch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Favonius Lance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>「渔获」</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西风长枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lithic Spear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>千岩长枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deathmatch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dragon's Bane</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>匣里灭辰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>决斗之枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blackcliff Pole</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑岩刺枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skyward Spine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Engulfing Lightning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天空之脊</t>
+  </si>
+  <si>
+    <t>薙草之稻光</t>
+  </si>
+  <si>
+    <t>薙草之稻光</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>护摩之杖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Staff of Homa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Primordial Jade Winged-Spear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>和璞鸢</t>
+  </si>
+  <si>
+    <t>Vortex Vanquisher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贯虹之槊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新手長槍</t>
+  </si>
+  <si>
+    <t>鐵尖槍</t>
+  </si>
+  <si>
+    <t>白纓槍</t>
+  </si>
+  <si>
+    <t>黑纓槍</t>
+  </si>
+  <si>
+    <t>鉞矛</t>
+  </si>
+  <si>
+    <t>流月針</t>
+  </si>
+  <si>
+    <t>試作星鐮</t>
+  </si>
+  <si>
+    <t>龍脊長槍</t>
+  </si>
+  <si>
+    <t>宗室獵槍</t>
+  </si>
+  <si>
+    <t>「漁獲」</t>
+  </si>
+  <si>
+    <t>決鬥之槍</t>
+  </si>
+  <si>
+    <t>匣裡滅辰</t>
+  </si>
+  <si>
+    <t>黑岩刺槍</t>
+  </si>
+  <si>
+    <t>護摩之杖</t>
+  </si>
+  <si>
+    <t>和璞鳶</t>
+  </si>
+  <si>
+    <t>貫虹之槊</t>
+  </si>
+  <si>
+    <t>千岩長槍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西風長槍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4908,8 +5988,16 @@
       <family val="3"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4943,6 +6031,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5045,7 +6139,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5169,6 +6263,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5187,12 +6287,24 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="44">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -6108,7 +7220,7 @@
     <sortCondition ref="B1:B10"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F8D7EDC0-D23C-46E6-811C-566418C3556F}" name="欄1" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{F8D7EDC0-D23C-46E6-811C-566418C3556F}" name="欄1" dataDxfId="43"/>
     <tableColumn id="2" xr3:uid="{94B273F2-2152-4C45-972D-7CF59CA686A0}" name="欄2"/>
     <tableColumn id="3" xr3:uid="{F572BF82-8FF2-44C3-A39B-FE676229F982}" name="欄3"/>
     <tableColumn id="4" xr3:uid="{5A22E185-B077-47FD-9521-482F30C2B555}" name="欄4"/>
@@ -6118,32 +7230,103 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{15464BD1-0DC5-4BD2-B6A8-59578FBE4A8A}" name="表格10" displayName="表格10" ref="A2:B12" totalsRowShown="0">
+  <autoFilter ref="A2:B12" xr:uid="{15464BD1-0DC5-4BD2-B6A8-59578FBE4A8A}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{20041694-57E1-40AE-B579-20BB0AB275DE}" name="EN"/>
+    <tableColumn id="2" xr3:uid="{242245F9-3664-4E59-B22D-647250C7E7EB}" name="Meaning'"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2C3F3A93-D8A8-48D6-BD9C-E5A8AC8A926D}" name="表格11" displayName="表格11" ref="G2:P29" totalsRowShown="0">
+  <autoFilter ref="G2:P29" xr:uid="{2C3F3A93-D8A8-48D6-BD9C-E5A8AC8A926D}"/>
+  <tableColumns count="10">
+    <tableColumn id="15" xr3:uid="{EC110DFF-2A53-4A12-917F-DB8D495934C1}" name="Id" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{1B03FF58-EB4E-451A-8EC1-D4134A8B6D80}" name="name"/>
+    <tableColumn id="16" xr3:uid="{A726EE41-BA0E-4B70-8EC7-E4C8743DA40C}" name="stars"/>
+    <tableColumn id="2" xr3:uid="{C7BCDEE6-8248-4490-A722-84B46743348F}" name="stat_1"/>
+    <tableColumn id="4" xr3:uid="{E16C4889-81DA-40EE-A51D-5FEBDFBA6AAB}" name="stat_2"/>
+    <tableColumn id="14" xr3:uid="{ECBBD842-58B3-4EBA-AD15-5DA1D2A984B4}" name="en_us"/>
+    <tableColumn id="6" xr3:uid="{B4FB6072-8F87-4972-96AA-67E5DC549501}" name="zh_hk"/>
+    <tableColumn id="7" xr3:uid="{06F6C5F3-C446-4632-A5EC-9A460BD0201E}" name="zh_cn"/>
+    <tableColumn id="8" xr3:uid="{4E6D7416-426E-4100-8D87-88A62E297113}" name="ru_ru"/>
+    <tableColumn id="9" xr3:uid="{E31400F2-D2D3-485C-86FB-8C62004B2DA4}" name="ja_jp"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E355504B-7F91-4471-BEAD-EE6C2F081A0F}" name="表格1113" displayName="表格1113" ref="R2:AA27" totalsRowShown="0">
+  <autoFilter ref="R2:AA27" xr:uid="{E355504B-7F91-4471-BEAD-EE6C2F081A0F}"/>
+  <tableColumns count="10">
+    <tableColumn id="15" xr3:uid="{FB1B7DA4-5014-4091-94BF-7267087285FF}" name="Id" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{1C4B0309-3595-428E-AEB3-A4ABA3F2DC48}" name="name"/>
+    <tableColumn id="16" xr3:uid="{82A5565C-A532-497E-A4FE-14FDBB1A800A}" name="stars"/>
+    <tableColumn id="2" xr3:uid="{B24E20AA-5F9D-4508-B069-501D4481B4FA}" name="stat_1"/>
+    <tableColumn id="4" xr3:uid="{363CDE87-44F3-41B3-A641-6A0BAE326AFD}" name="stat_2"/>
+    <tableColumn id="14" xr3:uid="{D1841425-8AFF-4744-8877-6A9AEB36AD7D}" name="en_us"/>
+    <tableColumn id="6" xr3:uid="{CAA95829-9C4E-4C22-AB4D-23733A10B06D}" name="zh_hk"/>
+    <tableColumn id="7" xr3:uid="{EDCAAD25-827C-4F94-9533-B331DFA30B5D}" name="zh_cn"/>
+    <tableColumn id="8" xr3:uid="{6779C416-2FD1-4BD8-8AC9-B0FBF79804CC}" name="ru_ru"/>
+    <tableColumn id="9" xr3:uid="{A5A2B046-1CCD-410B-97E5-D0875CCCE676}" name="ja_jp"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{555EA72C-B044-478B-A57F-131075C25D4E}" name="表格111314" displayName="表格111314" ref="AC2:AL23" totalsRowShown="0">
+  <autoFilter ref="AC2:AL23" xr:uid="{555EA72C-B044-478B-A57F-131075C25D4E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AC3:AL23">
+    <sortCondition ref="AC2:AC23"/>
+  </sortState>
+  <tableColumns count="10">
+    <tableColumn id="15" xr3:uid="{2E276206-0917-4B18-BD7F-B71BBBC4AD99}" name="Id" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{23C26060-0EF7-4D05-B388-5DC56E22C4C6}" name="name"/>
+    <tableColumn id="16" xr3:uid="{39C0C26D-2CFF-4D7C-833D-BB17362BEE82}" name="stars"/>
+    <tableColumn id="2" xr3:uid="{4AD8545C-F9D2-4056-AA83-35BB3D40E019}" name="stat_1"/>
+    <tableColumn id="4" xr3:uid="{B100F0F5-4E2D-4A8E-8A5D-EEA245575DD5}" name="stat_2"/>
+    <tableColumn id="14" xr3:uid="{0B4FB660-0EA7-4D6E-9C7D-DDE5048B1E90}" name="en_us"/>
+    <tableColumn id="6" xr3:uid="{AE4DDD75-680D-42EF-B3D9-C5B8A6116D30}" name="zh_hk"/>
+    <tableColumn id="7" xr3:uid="{EB44780A-0031-4CED-8D03-5AF0208E564A}" name="zh_cn"/>
+    <tableColumn id="8" xr3:uid="{EE0FA7E2-4EA6-451A-A2A0-D17ED1E87C23}" name="ru_ru"/>
+    <tableColumn id="9" xr3:uid="{6D9B5B63-BE08-431E-A2E4-2CD8A403EBE7}" name="ja_jp"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{473CDE15-4806-4BE7-AA96-B40FBCF102DE}" name="表格3" displayName="表格3" ref="L1:P42" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{473CDE15-4806-4BE7-AA96-B40FBCF102DE}" name="表格3" displayName="表格3" ref="L1:P42" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <autoFilter ref="L1:P42" xr:uid="{473CDE15-4806-4BE7-AA96-B40FBCF102DE}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6AC5CD60-6F10-4D8C-B6C5-750AC51A1851}" name="欄1" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{E52E40DB-9D86-4DA7-8F40-CABBC5682667}" name="欄2" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{CFC9CC74-0D9A-4B80-A217-216C55C87EA6}" name="欄3" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{D0E41185-D8BF-4874-96C3-C51512AA32F0}" name="欄4" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{20534908-AE06-4E11-9C48-72752018E6AB}" name="欄5" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{6AC5CD60-6F10-4D8C-B6C5-750AC51A1851}" name="欄1" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{E52E40DB-9D86-4DA7-8F40-CABBC5682667}" name="欄2" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{CFC9CC74-0D9A-4B80-A217-216C55C87EA6}" name="欄3" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{D0E41185-D8BF-4874-96C3-C51512AA32F0}" name="欄4" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{20534908-AE06-4E11-9C48-72752018E6AB}" name="欄5" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2A78286-176C-4F13-BA46-F1CB954EBA8A}" name="表格3_5" displayName="表格3_5" ref="R1:V42" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2A78286-176C-4F13-BA46-F1CB954EBA8A}" name="表格3_5" displayName="表格3_5" ref="R1:V42" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="R1:V42" xr:uid="{C2A78286-176C-4F13-BA46-F1CB954EBA8A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R2:V42">
     <sortCondition ref="S1:S42"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C3672042-00E8-484A-B1F8-9547D9C24F1C}" name="欄1" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{14098B71-1643-45FE-8C3A-4EDD9592D446}" name="欄2" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{1F334A15-498B-4BAF-88F3-1B08C566CC0B}" name="欄3" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{163E8FDE-C6FA-4860-BB56-DCA54D72A676}" name="欄4" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{5CD6E9E9-6BDB-41C9-9675-C6B3F6FF8062}" name="欄5" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{C3672042-00E8-484A-B1F8-9547D9C24F1C}" name="欄1" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{14098B71-1643-45FE-8C3A-4EDD9592D446}" name="欄2" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{1F334A15-498B-4BAF-88F3-1B08C566CC0B}" name="欄3" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{163E8FDE-C6FA-4860-BB56-DCA54D72A676}" name="欄4" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{5CD6E9E9-6BDB-41C9-9675-C6B3F6FF8062}" name="欄5" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6174,9 +7357,9 @@
     <tableColumn id="10" xr3:uid="{2CA12209-BEC1-446B-837E-3625B66D6479}" name="欄6"/>
     <tableColumn id="11" xr3:uid="{2F7BDED2-E982-465A-B8B9-13C77DFFF140}" name="isComingSoon"/>
     <tableColumn id="12" xr3:uid="{8ED078E3-D2E5-4368-B7AA-86F09197E483}" name="欄7"/>
-    <tableColumn id="13" xr3:uid="{F499B208-A2C0-40A2-AF4F-08B2864D50A5}" name="Nation" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{F499B208-A2C0-40A2-AF4F-08B2864D50A5}" name="Nation" dataDxfId="22"/>
     <tableColumn id="14" xr3:uid="{E4841D03-A89B-4225-BC6E-DAB79E4F69BA}" name="欄8"/>
-    <tableColumn id="15" xr3:uid="{0859A80F-96D6-43FB-963F-2975A79D04A2}" name="Sex" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{0859A80F-96D6-43FB-963F-2975A79D04A2}" name="Sex" dataDxfId="21"/>
     <tableColumn id="16" xr3:uid="{1894B40B-FC5A-40C6-8A31-D990D4DCBEDA}" name="欄9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6202,9 +7385,9 @@
     <tableColumn id="10" xr3:uid="{A1C3925A-BC1D-49AD-BD0A-C0C6FF86710C}" name="欄8"/>
     <tableColumn id="11" xr3:uid="{DDCFEB9E-5DA7-44E3-8B6E-E882B0296DBE}" name="欄10"/>
     <tableColumn id="12" xr3:uid="{9025A34E-B09A-478F-ACD3-F4808D9018A8}" name="欄11"/>
-    <tableColumn id="13" xr3:uid="{BC2704BE-C18D-494E-9323-E6CEC40CCBDD}" name="欄12" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{BC2704BE-C18D-494E-9323-E6CEC40CCBDD}" name="欄12" dataDxfId="20"/>
     <tableColumn id="14" xr3:uid="{99CDB4FB-5A98-4A92-9B3A-D8A142CD4650}" name="欄13"/>
-    <tableColumn id="15" xr3:uid="{57901587-33CB-4B1B-9D1A-29869E5D51CF}" name="欄14" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{57901587-33CB-4B1B-9D1A-29869E5D51CF}" name="欄14" dataDxfId="19"/>
     <tableColumn id="16" xr3:uid="{E15460D2-39A1-4749-A0BC-79D78BDC80A3}" name="欄9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6215,9 +7398,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2F8C9CD3-6807-4BB1-912C-534D61040DE2}" name="表格5" displayName="表格5" ref="A2:C92" totalsRowShown="0">
   <autoFilter ref="A2:C92" xr:uid="{2F8C9CD3-6807-4BB1-912C-534D61040DE2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4D933B04-2089-4C42-B0F5-9CCF437372DE}" name="Lvl" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{19F425B7-5DDF-49D7-AF9A-C7488228FC37}" name="EXP" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{EBC5B7AC-235A-443F-9457-36203EB4C657}" name="Mora" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{4D933B04-2089-4C42-B0F5-9CCF437372DE}" name="Lvl" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{19F425B7-5DDF-49D7-AF9A-C7488228FC37}" name="EXP" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{EBC5B7AC-235A-443F-9457-36203EB4C657}" name="Mora" dataDxfId="16">
       <calculatedColumnFormula>表格5[[#This Row],[EXP]]/5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6226,10 +7409,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3CBCC354-20AF-4B90-B32B-2773B06C4903}" name="表格7" displayName="表格7" ref="L2:V9" totalsRowShown="0" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3CBCC354-20AF-4B90-B32B-2773B06C4903}" name="表格7" displayName="表格7" ref="L2:V9" totalsRowShown="0" tableBorderDxfId="15">
   <autoFilter ref="L2:V9" xr:uid="{3CBCC354-20AF-4B90-B32B-2773B06C4903}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{445C1D55-89FB-45DA-AC14-C3B2291AD18C}" name="Lvl" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{445C1D55-89FB-45DA-AC14-C3B2291AD18C}" name="Lvl" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{D85ADDA0-5697-4B45-B253-D28D12138887}" name="silver"/>
     <tableColumn id="3" xr3:uid="{C74453EA-1392-420B-9F6D-B70ED17F5F04}" name="fragment"/>
     <tableColumn id="4" xr3:uid="{4E395841-CCE4-4125-A549-76820121865B}" name="chunk"/>
@@ -6246,10 +7429,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B6F67A92-13C6-452B-B533-7A6CE4B956BC}" name="表格7_9" displayName="表格7_9" ref="L23:U33" totalsRowShown="0" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B6F67A92-13C6-452B-B533-7A6CE4B956BC}" name="表格7_9" displayName="表格7_9" ref="L23:U33" totalsRowShown="0" tableBorderDxfId="13">
   <autoFilter ref="L23:U33" xr:uid="{B6F67A92-13C6-452B-B533-7A6CE4B956BC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{E5F80E02-005D-4CE6-938B-BC3A3F902FA9}" name="Lvl" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{E5F80E02-005D-4CE6-938B-BC3A3F902FA9}" name="Lvl" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{63946B89-AD80-421F-843F-3ACEB5116A1F}" name="teach"/>
     <tableColumn id="3" xr3:uid="{95661BC4-9F13-4054-AFE8-53C0C9C938DF}" name="guide"/>
     <tableColumn id="4" xr3:uid="{CC0A828D-0AE2-4065-B058-C2C341F047E4}" name="phi"/>
@@ -6265,19 +7448,19 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BC3DCDF1-850C-4450-AFF2-19B7D92E1A07}" name="表格9" displayName="表格9" ref="L50:S91" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BC3DCDF1-850C-4450-AFF2-19B7D92E1A07}" name="表格9" displayName="表格9" ref="L50:S91" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L51:T86">
     <sortCondition ref="L50:L86"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="9" xr3:uid="{6C52EE62-FF4B-4DE8-83C0-D6436E18DD9A}" name="ID" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{6C52EE62-FF4B-4DE8-83C0-D6436E18DD9A}" name="ID" dataDxfId="9"/>
     <tableColumn id="1" xr3:uid="{6B0882EA-DCCC-4EC2-A448-3DA915481575}" name="CharName"/>
-    <tableColumn id="2" xr3:uid="{E53A3D14-8402-47E5-B585-0960C1B3C866}" name="Crystal" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{6F35CFC6-EB53-4FD8-9991-84FD8CE6220B}" name="Boss" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{17B35194-9BF4-42AC-965C-670DDA3FA254}" name="Local" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{8827F259-32C5-474B-9C18-649FDAECC3B3}" name="Common" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{9386E62E-DB69-43C8-90CB-7E2B6F05B2C2}" name="Talent-Book" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{EB22D77C-1EAF-4FC1-A992-7476EECA02BA}" name="Talent-Boss" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{E53A3D14-8402-47E5-B585-0960C1B3C866}" name="Crystal" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{6F35CFC6-EB53-4FD8-9991-84FD8CE6220B}" name="Boss" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{17B35194-9BF4-42AC-965C-670DDA3FA254}" name="Local" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{8827F259-32C5-474B-9C18-649FDAECC3B3}" name="Common" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{9386E62E-DB69-43C8-90CB-7E2B6F05B2C2}" name="Talent-Book" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{EB22D77C-1EAF-4FC1-A992-7476EECA02BA}" name="Talent-Boss" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8849,7 +10032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD46B98-C1E0-46DC-B117-82EFF581F8D6}">
   <dimension ref="A1:P95"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A53" sqref="A53:C95"/>
     </sheetView>
   </sheetViews>
@@ -11070,22 +12253,22 @@
     </row>
     <row r="50" spans="1:16" ht="17.25" thickBot="1"/>
     <row r="51" spans="1:16" s="21" customFormat="1" ht="26.25" thickBot="1">
-      <c r="D51" s="41" t="s">
+      <c r="D51" s="43" t="s">
         <v>605</v>
       </c>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="41" t="s">
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="43" t="s">
         <v>604</v>
       </c>
-      <c r="K51" s="42"/>
-      <c r="L51" s="42"/>
-      <c r="M51" s="42"/>
-      <c r="N51" s="42"/>
-      <c r="O51" s="43"/>
+      <c r="K51" s="44"/>
+      <c r="L51" s="44"/>
+      <c r="M51" s="44"/>
+      <c r="N51" s="44"/>
+      <c r="O51" s="45"/>
     </row>
     <row r="52" spans="1:16">
       <c r="A52" t="s">
@@ -19831,7 +21014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DDF792-EDA2-41C8-9FF9-80AF9A857C2E}">
   <dimension ref="A1:AK278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G191" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="G196" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P203" sqref="P203"/>
     </sheetView>
   </sheetViews>
@@ -19863,43 +21046,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="32.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>837</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="L1" s="45" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="L1" s="47" t="s">
         <v>860</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
     </row>
     <row r="2" spans="1:34">
       <c r="A2" s="25" t="s">
@@ -20013,14 +21196,14 @@
       <c r="V3">
         <v>0</v>
       </c>
-      <c r="Z3" s="46" t="s">
+      <c r="Z3" s="48" t="s">
         <v>873</v>
       </c>
-      <c r="AA3" s="46"/>
-      <c r="AB3" s="46"/>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="46"/>
-      <c r="AE3" s="46"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="48"/>
+      <c r="AE3" s="48"/>
     </row>
     <row r="4" spans="1:34">
       <c r="A4" s="26">
@@ -20087,12 +21270,12 @@
       <c r="V4">
         <v>20000</v>
       </c>
-      <c r="Z4" s="46"/>
-      <c r="AA4" s="46"/>
-      <c r="AB4" s="46"/>
-      <c r="AC4" s="46"/>
-      <c r="AD4" s="46"/>
-      <c r="AE4" s="46"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="48"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="48"/>
+      <c r="AE4" s="48"/>
     </row>
     <row r="5" spans="1:34">
       <c r="A5" s="26">
@@ -20159,12 +21342,12 @@
       <c r="V5">
         <v>40000</v>
       </c>
-      <c r="Z5" s="46"/>
-      <c r="AA5" s="46"/>
-      <c r="AB5" s="46"/>
-      <c r="AC5" s="46"/>
-      <c r="AD5" s="46"/>
-      <c r="AE5" s="46"/>
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="48"/>
+      <c r="AB5" s="48"/>
+      <c r="AC5" s="48"/>
+      <c r="AD5" s="48"/>
+      <c r="AE5" s="48"/>
     </row>
     <row r="6" spans="1:34">
       <c r="A6" s="26">
@@ -20231,12 +21414,12 @@
       <c r="V6">
         <v>60000</v>
       </c>
-      <c r="Z6" s="46"/>
-      <c r="AA6" s="46"/>
-      <c r="AB6" s="46"/>
-      <c r="AC6" s="46"/>
-      <c r="AD6" s="46"/>
-      <c r="AE6" s="46"/>
+      <c r="Z6" s="48"/>
+      <c r="AA6" s="48"/>
+      <c r="AB6" s="48"/>
+      <c r="AC6" s="48"/>
+      <c r="AD6" s="48"/>
+      <c r="AE6" s="48"/>
     </row>
     <row r="7" spans="1:34">
       <c r="A7" s="26">
@@ -21453,31 +22636,31 @@
         <f>表格5[[#This Row],[Mora]]&amp;"},"</f>
         <v>2755},</v>
       </c>
-      <c r="L22" s="44" t="s">
+      <c r="L22" s="46" t="s">
         <v>863</v>
       </c>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="44"/>
-      <c r="Q22" s="44"/>
-      <c r="R22" s="44"/>
-      <c r="S22" s="44"/>
-      <c r="T22" s="44"/>
-      <c r="U22" s="44"/>
-      <c r="V22" s="44"/>
-      <c r="W22" s="44"/>
-      <c r="X22" s="44"/>
-      <c r="Y22" s="44"/>
-      <c r="Z22" s="44"/>
-      <c r="AA22" s="44"/>
-      <c r="AB22" s="44"/>
-      <c r="AC22" s="44"/>
-      <c r="AD22" s="44"/>
-      <c r="AE22" s="44"/>
-      <c r="AF22" s="44"/>
-      <c r="AG22" s="44"/>
-      <c r="AH22" s="44"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="46"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="46"/>
+      <c r="S22" s="46"/>
+      <c r="T22" s="46"/>
+      <c r="U22" s="46"/>
+      <c r="V22" s="46"/>
+      <c r="W22" s="46"/>
+      <c r="X22" s="46"/>
+      <c r="Y22" s="46"/>
+      <c r="Z22" s="46"/>
+      <c r="AA22" s="46"/>
+      <c r="AB22" s="46"/>
+      <c r="AC22" s="46"/>
+      <c r="AD22" s="46"/>
+      <c r="AE22" s="46"/>
+      <c r="AF22" s="46"/>
+      <c r="AG22" s="46"/>
+      <c r="AH22" s="46"/>
     </row>
     <row r="23" spans="1:34">
       <c r="A23" s="26">
@@ -23399,33 +24582,33 @@
         <f>表格5[[#This Row],[Mora]]&amp;"},"</f>
         <v>12255},</v>
       </c>
-      <c r="L49" s="44" t="s">
+      <c r="L49" s="46" t="s">
         <v>875</v>
       </c>
-      <c r="M49" s="44"/>
-      <c r="N49" s="44"/>
-      <c r="O49" s="44"/>
-      <c r="P49" s="44"/>
-      <c r="Q49" s="44"/>
-      <c r="R49" s="44"/>
-      <c r="S49" s="44"/>
-      <c r="T49" s="44"/>
-      <c r="U49" s="44"/>
-      <c r="V49" s="44"/>
-      <c r="W49" s="44"/>
-      <c r="X49" s="44"/>
-      <c r="Y49" s="44"/>
-      <c r="Z49" s="44"/>
-      <c r="AA49" s="44"/>
-      <c r="AB49" s="44"/>
-      <c r="AC49" s="44"/>
-      <c r="AD49" s="44"/>
-      <c r="AE49" s="44"/>
-      <c r="AF49" s="44"/>
-      <c r="AG49" s="44"/>
-      <c r="AH49" s="44"/>
-      <c r="AI49" s="44"/>
-      <c r="AJ49" s="44"/>
+      <c r="M49" s="46"/>
+      <c r="N49" s="46"/>
+      <c r="O49" s="46"/>
+      <c r="P49" s="46"/>
+      <c r="Q49" s="46"/>
+      <c r="R49" s="46"/>
+      <c r="S49" s="46"/>
+      <c r="T49" s="46"/>
+      <c r="U49" s="46"/>
+      <c r="V49" s="46"/>
+      <c r="W49" s="46"/>
+      <c r="X49" s="46"/>
+      <c r="Y49" s="46"/>
+      <c r="Z49" s="46"/>
+      <c r="AA49" s="46"/>
+      <c r="AB49" s="46"/>
+      <c r="AC49" s="46"/>
+      <c r="AD49" s="46"/>
+      <c r="AE49" s="46"/>
+      <c r="AF49" s="46"/>
+      <c r="AG49" s="46"/>
+      <c r="AH49" s="46"/>
+      <c r="AI49" s="46"/>
+      <c r="AJ49" s="46"/>
       <c r="AK49" s="21"/>
     </row>
     <row r="50" spans="1:37">
@@ -36600,4 +37783,1688 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4FB002-A857-4FB3-9B85-E1B286490B83}">
+  <dimension ref="A1:AM29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AB18" sqref="AB18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="13.875" customWidth="1"/>
+    <col min="6" max="6" width="9" style="42"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="42"/>
+    <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9" style="42"/>
+    <col min="30" max="30" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" ht="25.5" customHeight="1">
+      <c r="A1" s="49" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="G1" s="49" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="R1" s="49" t="s">
+        <v>1376</v>
+      </c>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AC1" s="49" t="s">
+        <v>1478</v>
+      </c>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="49"/>
+      <c r="AG1" s="49"/>
+      <c r="AH1" s="49"/>
+      <c r="AI1" s="49"/>
+      <c r="AJ1" s="49"/>
+      <c r="AK1" s="49"/>
+      <c r="AL1" s="49"/>
+    </row>
+    <row r="2" spans="1:38">
+      <c r="A2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1235</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1319</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1254</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1255</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1264</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1256</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1257</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1259</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1319</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1254</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1255</v>
+      </c>
+      <c r="W2" t="s">
+        <v>1264</v>
+      </c>
+      <c r="X2" t="s">
+        <v>1256</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>1257</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>1259</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>1319</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>1254</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>1255</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>1264</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>1256</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>1257</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38">
+      <c r="A3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="G3" s="17">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1265</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1321</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1249</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R3" s="17">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="W3" t="s">
+        <v>1406</v>
+      </c>
+      <c r="X3" t="s">
+        <v>1455</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>1377</v>
+      </c>
+      <c r="AC3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>1479</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>1479</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>1523</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38">
+      <c r="A4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G4" s="17">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1266</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1293</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1353</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1327</v>
+      </c>
+      <c r="R4" s="17">
+        <v>2</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1431</v>
+      </c>
+      <c r="W4" t="s">
+        <v>1407</v>
+      </c>
+      <c r="X4" t="s">
+        <v>1456</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>1378</v>
+      </c>
+      <c r="AC4" s="17">
+        <v>2</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>1481</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>1481</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>1524</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38">
+      <c r="A5" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1237</v>
+      </c>
+      <c r="G5" s="17">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1267</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1323</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1294</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1354</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1328</v>
+      </c>
+      <c r="R5" s="17">
+        <v>3</v>
+      </c>
+      <c r="S5" t="s">
+        <v>1432</v>
+      </c>
+      <c r="W5" t="s">
+        <v>1408</v>
+      </c>
+      <c r="X5" t="s">
+        <v>1457</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>1380</v>
+      </c>
+      <c r="AC5" s="17">
+        <v>3</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>1483</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>1483</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>1525</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38">
+      <c r="A6" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G6" s="17">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1268</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1321</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1295</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1248</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1329</v>
+      </c>
+      <c r="R6" s="17">
+        <v>4</v>
+      </c>
+      <c r="S6" t="s">
+        <v>1433</v>
+      </c>
+      <c r="W6" t="s">
+        <v>1409</v>
+      </c>
+      <c r="X6" t="s">
+        <v>1379</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>1381</v>
+      </c>
+      <c r="AC6" s="17">
+        <v>4</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>1486</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>1486</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38">
+      <c r="A7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1232</v>
+      </c>
+      <c r="G7" s="17">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1269</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1247</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1296</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1355</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1330</v>
+      </c>
+      <c r="R7" s="17">
+        <v>5</v>
+      </c>
+      <c r="S7" t="s">
+        <v>1434</v>
+      </c>
+      <c r="W7" t="s">
+        <v>1383</v>
+      </c>
+      <c r="X7" t="s">
+        <v>1458</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>1382</v>
+      </c>
+      <c r="AC7" s="17">
+        <v>5</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>1487</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>1487</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>1527</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38">
+      <c r="A8" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1233</v>
+      </c>
+      <c r="G8" s="17">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1270</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>124</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1297</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1356</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1331</v>
+      </c>
+      <c r="R8" s="17">
+        <v>6</v>
+      </c>
+      <c r="S8" t="s">
+        <v>1435</v>
+      </c>
+      <c r="W8" t="s">
+        <v>1410</v>
+      </c>
+      <c r="X8" t="s">
+        <v>1477</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>1476</v>
+      </c>
+      <c r="AC8" s="17">
+        <v>6</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>1489</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>1489</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>1528</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38">
+      <c r="A9" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1234</v>
+      </c>
+      <c r="G9" s="17">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1271</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1245</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1298</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1357</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1332</v>
+      </c>
+      <c r="R9" s="17">
+        <v>7</v>
+      </c>
+      <c r="S9" t="s">
+        <v>1436</v>
+      </c>
+      <c r="W9" t="s">
+        <v>1411</v>
+      </c>
+      <c r="X9" t="s">
+        <v>1459</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>1475</v>
+      </c>
+      <c r="AC9" s="17">
+        <v>7</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>1491</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>1491</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>1529</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38">
+      <c r="A10" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1244</v>
+      </c>
+      <c r="G10" s="17">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1272</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1245</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1299</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1333</v>
+      </c>
+      <c r="R10" s="17">
+        <v>8</v>
+      </c>
+      <c r="S10" t="s">
+        <v>1437</v>
+      </c>
+      <c r="W10" t="s">
+        <v>1412</v>
+      </c>
+      <c r="X10" t="s">
+        <v>1460</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>1385</v>
+      </c>
+      <c r="AC10" s="17">
+        <v>8</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>1493</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>1493</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>1494</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38">
+      <c r="A11" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1262</v>
+      </c>
+      <c r="G11" s="17">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1273</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1321</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1300</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1359</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1334</v>
+      </c>
+      <c r="R11" s="17">
+        <v>9</v>
+      </c>
+      <c r="S11" t="s">
+        <v>1438</v>
+      </c>
+      <c r="W11" t="s">
+        <v>1413</v>
+      </c>
+      <c r="X11" t="s">
+        <v>1461</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>1386</v>
+      </c>
+      <c r="AC11" s="17">
+        <v>9</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>1496</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>1496</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>1530</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38">
+      <c r="A12" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G12" s="17">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1274</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1247</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1301</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1360</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1335</v>
+      </c>
+      <c r="R12" s="17">
+        <v>10</v>
+      </c>
+      <c r="S12" t="s">
+        <v>1439</v>
+      </c>
+      <c r="W12" t="s">
+        <v>1414</v>
+      </c>
+      <c r="X12" t="s">
+        <v>1462</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>1387</v>
+      </c>
+      <c r="AC12" s="17">
+        <v>10</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>1498</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>1498</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>1531</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38">
+      <c r="G13" s="17">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1275</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1323</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1302</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1361</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1336</v>
+      </c>
+      <c r="R13" s="17">
+        <v>11</v>
+      </c>
+      <c r="S13" t="s">
+        <v>1440</v>
+      </c>
+      <c r="W13" t="s">
+        <v>1415</v>
+      </c>
+      <c r="X13" t="s">
+        <v>1463</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>1388</v>
+      </c>
+      <c r="AC13" s="17">
+        <v>11</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>1500</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>1500</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>1532</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38">
+      <c r="G14" s="17">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1276</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1247</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1303</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1362</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1337</v>
+      </c>
+      <c r="R14" s="17">
+        <v>12</v>
+      </c>
+      <c r="S14" t="s">
+        <v>1441</v>
+      </c>
+      <c r="W14" t="s">
+        <v>1416</v>
+      </c>
+      <c r="X14" t="s">
+        <v>1464</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>1389</v>
+      </c>
+      <c r="AC14" s="17">
+        <v>12</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>1501</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>1501</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>1540</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38">
+      <c r="G15" s="17">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1277</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1321</v>
+      </c>
+      <c r="K15" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L15" t="s">
+        <v>1304</v>
+      </c>
+      <c r="M15" t="s">
+        <v>1363</v>
+      </c>
+      <c r="N15" t="s">
+        <v>1338</v>
+      </c>
+      <c r="R15" s="17">
+        <v>13</v>
+      </c>
+      <c r="S15" t="s">
+        <v>1442</v>
+      </c>
+      <c r="W15" t="s">
+        <v>1417</v>
+      </c>
+      <c r="X15" t="s">
+        <v>1465</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>1390</v>
+      </c>
+      <c r="AC15" s="17">
+        <v>13</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>1504</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>1504</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>1539</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38">
+      <c r="G16" s="17">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1278</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1323</v>
+      </c>
+      <c r="K16" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L16" t="s">
+        <v>1305</v>
+      </c>
+      <c r="M16" t="s">
+        <v>1364</v>
+      </c>
+      <c r="N16" t="s">
+        <v>1339</v>
+      </c>
+      <c r="R16" s="17">
+        <v>14</v>
+      </c>
+      <c r="S16" t="s">
+        <v>1443</v>
+      </c>
+      <c r="W16" t="s">
+        <v>1418</v>
+      </c>
+      <c r="X16" t="s">
+        <v>1466</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>1391</v>
+      </c>
+      <c r="AC16" s="17">
+        <v>14</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>1506</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>1506</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>1533</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="17" spans="7:36">
+      <c r="G17" s="17">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1279</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1324</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1306</v>
+      </c>
+      <c r="M17" t="s">
+        <v>1365</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1341</v>
+      </c>
+      <c r="R17" s="17">
+        <v>15</v>
+      </c>
+      <c r="S17" t="s">
+        <v>1444</v>
+      </c>
+      <c r="W17" t="s">
+        <v>1419</v>
+      </c>
+      <c r="X17" t="s">
+        <v>1392</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>1393</v>
+      </c>
+      <c r="AC17" s="17">
+        <v>15</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>1507</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>1507</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>1534</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="18" spans="7:36">
+      <c r="G18" s="17">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1280</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1322</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L18" t="s">
+        <v>1307</v>
+      </c>
+      <c r="M18" t="s">
+        <v>1366</v>
+      </c>
+      <c r="N18" t="s">
+        <v>1342</v>
+      </c>
+      <c r="R18" s="17">
+        <v>16</v>
+      </c>
+      <c r="S18" t="s">
+        <v>1445</v>
+      </c>
+      <c r="W18" t="s">
+        <v>1420</v>
+      </c>
+      <c r="X18" t="s">
+        <v>1467</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>1394</v>
+      </c>
+      <c r="AC18" s="17">
+        <v>16</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>1510</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>1510</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>1535</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="19" spans="7:36">
+      <c r="G19" s="17">
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1281</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1321</v>
+      </c>
+      <c r="K19" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1308</v>
+      </c>
+      <c r="M19" t="s">
+        <v>1367</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1343</v>
+      </c>
+      <c r="R19" s="17">
+        <v>17</v>
+      </c>
+      <c r="S19" t="s">
+        <v>1446</v>
+      </c>
+      <c r="W19" t="s">
+        <v>1421</v>
+      </c>
+      <c r="X19" t="s">
+        <v>1468</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>1395</v>
+      </c>
+      <c r="AC19" s="17">
+        <v>17</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>1512</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>1512</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>1514</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="20" spans="7:36">
+      <c r="G20" s="17">
+        <v>18</v>
+      </c>
+      <c r="H20" t="s">
+        <v>1282</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="J20" t="s">
+        <v>1245</v>
+      </c>
+      <c r="K20" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L20" t="s">
+        <v>1309</v>
+      </c>
+      <c r="M20" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N20" t="s">
+        <v>1344</v>
+      </c>
+      <c r="R20" s="17">
+        <v>18</v>
+      </c>
+      <c r="S20" t="s">
+        <v>1447</v>
+      </c>
+      <c r="W20" t="s">
+        <v>1422</v>
+      </c>
+      <c r="X20" t="s">
+        <v>1469</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>1396</v>
+      </c>
+      <c r="AC20" s="17">
+        <v>18</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>1513</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>1513</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>1515</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="21" spans="7:36">
+      <c r="G21" s="17">
+        <v>19</v>
+      </c>
+      <c r="H21" t="s">
+        <v>1283</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21" t="s">
+        <v>124</v>
+      </c>
+      <c r="K21" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L21" t="s">
+        <v>1310</v>
+      </c>
+      <c r="M21" t="s">
+        <v>1369</v>
+      </c>
+      <c r="N21" t="s">
+        <v>1345</v>
+      </c>
+      <c r="R21" s="17">
+        <v>19</v>
+      </c>
+      <c r="S21" t="s">
+        <v>1448</v>
+      </c>
+      <c r="W21" t="s">
+        <v>1423</v>
+      </c>
+      <c r="X21" t="s">
+        <v>1470</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>1397</v>
+      </c>
+      <c r="AC21" s="17">
+        <v>19</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>1518</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>1518</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>1536</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="22" spans="7:36">
+      <c r="G22" s="17">
+        <v>20</v>
+      </c>
+      <c r="H22" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22" t="s">
+        <v>1245</v>
+      </c>
+      <c r="K22" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L22" t="s">
+        <v>1311</v>
+      </c>
+      <c r="M22" t="s">
+        <v>1370</v>
+      </c>
+      <c r="N22" t="s">
+        <v>1340</v>
+      </c>
+      <c r="R22" s="17">
+        <v>20</v>
+      </c>
+      <c r="S22" t="s">
+        <v>1449</v>
+      </c>
+      <c r="W22" t="s">
+        <v>1424</v>
+      </c>
+      <c r="X22" t="s">
+        <v>1471</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>1398</v>
+      </c>
+      <c r="AC22" s="17">
+        <v>20</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>1519</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>1519</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>1537</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="23" spans="7:36">
+      <c r="G23" s="17">
+        <v>21</v>
+      </c>
+      <c r="H23" t="s">
+        <v>1285</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23" t="s">
+        <v>1245</v>
+      </c>
+      <c r="K23" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L23" t="s">
+        <v>1312</v>
+      </c>
+      <c r="M23" t="s">
+        <v>1250</v>
+      </c>
+      <c r="N23" t="s">
+        <v>1346</v>
+      </c>
+      <c r="R23" s="17">
+        <v>21</v>
+      </c>
+      <c r="S23" t="s">
+        <v>1450</v>
+      </c>
+      <c r="W23" t="s">
+        <v>1425</v>
+      </c>
+      <c r="X23" t="s">
+        <v>1472</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>1399</v>
+      </c>
+      <c r="AC23" s="17">
+        <v>21</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>1521</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>1521</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>1538</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="24" spans="7:36">
+      <c r="G24" s="17">
+        <v>22</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1286</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24" t="s">
+        <v>1321</v>
+      </c>
+      <c r="K24" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L24" t="s">
+        <v>1313</v>
+      </c>
+      <c r="M24" t="s">
+        <v>1251</v>
+      </c>
+      <c r="N24" t="s">
+        <v>1347</v>
+      </c>
+      <c r="R24" s="17">
+        <v>22</v>
+      </c>
+      <c r="S24" t="s">
+        <v>1451</v>
+      </c>
+      <c r="W24" t="s">
+        <v>1426</v>
+      </c>
+      <c r="X24" t="s">
+        <v>1400</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>1401</v>
+      </c>
+      <c r="AC24" s="17"/>
+    </row>
+    <row r="25" spans="7:36">
+      <c r="G25" s="17">
+        <v>23</v>
+      </c>
+      <c r="H25" t="s">
+        <v>1287</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="J25" t="s">
+        <v>1321</v>
+      </c>
+      <c r="K25" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L25" t="s">
+        <v>1314</v>
+      </c>
+      <c r="M25" t="s">
+        <v>1371</v>
+      </c>
+      <c r="N25" t="s">
+        <v>1348</v>
+      </c>
+      <c r="R25" s="17">
+        <v>23</v>
+      </c>
+      <c r="S25" t="s">
+        <v>1452</v>
+      </c>
+      <c r="W25" t="s">
+        <v>1427</v>
+      </c>
+      <c r="X25" t="s">
+        <v>1473</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>1402</v>
+      </c>
+      <c r="AC25" s="17"/>
+    </row>
+    <row r="26" spans="7:36">
+      <c r="G26" s="17">
+        <v>24</v>
+      </c>
+      <c r="H26" t="s">
+        <v>1288</v>
+      </c>
+      <c r="I26">
+        <v>4</v>
+      </c>
+      <c r="J26" t="s">
+        <v>1247</v>
+      </c>
+      <c r="K26" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L26" t="s">
+        <v>1315</v>
+      </c>
+      <c r="M26" t="s">
+        <v>1372</v>
+      </c>
+      <c r="N26" t="s">
+        <v>1349</v>
+      </c>
+      <c r="R26" s="17">
+        <v>24</v>
+      </c>
+      <c r="S26" t="s">
+        <v>1453</v>
+      </c>
+      <c r="W26" t="s">
+        <v>1428</v>
+      </c>
+      <c r="X26" t="s">
+        <v>1474</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>1403</v>
+      </c>
+      <c r="AC26" s="17"/>
+    </row>
+    <row r="27" spans="7:36">
+      <c r="G27" s="17">
+        <v>25</v>
+      </c>
+      <c r="H27" t="s">
+        <v>1289</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27" t="s">
+        <v>1324</v>
+      </c>
+      <c r="K27" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L27" t="s">
+        <v>1316</v>
+      </c>
+      <c r="M27" t="s">
+        <v>1373</v>
+      </c>
+      <c r="N27" t="s">
+        <v>1350</v>
+      </c>
+      <c r="R27" s="17">
+        <v>25</v>
+      </c>
+      <c r="S27" t="s">
+        <v>1454</v>
+      </c>
+      <c r="W27" t="s">
+        <v>1429</v>
+      </c>
+      <c r="X27" t="s">
+        <v>1404</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>1405</v>
+      </c>
+      <c r="AC27" s="17"/>
+    </row>
+    <row r="28" spans="7:36">
+      <c r="G28" s="17">
+        <v>26</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1290</v>
+      </c>
+      <c r="I28">
+        <v>4</v>
+      </c>
+      <c r="J28" t="s">
+        <v>1321</v>
+      </c>
+      <c r="K28" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L28" t="s">
+        <v>1317</v>
+      </c>
+      <c r="M28" t="s">
+        <v>1374</v>
+      </c>
+      <c r="N28" t="s">
+        <v>1351</v>
+      </c>
+      <c r="R28" s="17"/>
+    </row>
+    <row r="29" spans="7:36">
+      <c r="G29" s="17">
+        <v>27</v>
+      </c>
+      <c r="H29" t="s">
+        <v>1291</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1263</v>
+      </c>
+      <c r="K29" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L29" t="s">
+        <v>1318</v>
+      </c>
+      <c r="M29" t="s">
+        <v>1375</v>
+      </c>
+      <c r="N29" t="s">
+        <v>1352</v>
+      </c>
+      <c r="R29" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G1:P1"/>
+    <mergeCell ref="R1:AA1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="AC1:AL1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>